<commit_message>
Deal management UI testcases
</commit_message>
<xml_diff>
--- a/DM/databank/banking/deal_management/BANK_82_6_Test_43707_V1.xlsx
+++ b/DM/databank/banking/deal_management/BANK_82_6_Test_43707_V1.xlsx
@@ -105,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1807" uniqueCount="631">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1887" uniqueCount="711">
   <si>
     <t>SQ. NO.</t>
   </si>
@@ -2006,6 +2006,246 @@
   </si>
   <si>
     <t>{"C1-DealPriceAsgnCommitmentsREST":{"dealId":"1434978218","modelId":"6036438079","entityId":"8797366188","entityType":"PERS","pricingAndCommitmentsDetails":{"entityId":"8797366188","entityType":"PERS","entityIdentifierValue":"Reg_BANK_82_EPER_001","entityIdentifierType":"COREG","entityDivision":"IND","pricingDetails":{"priceAsgnId":"6060014089","actionFlag":"UPD","priceItemCode":"NPI_024","priceItemDescription":"Price Item NPI_024","pricingStatus":"PRPD","priceCurrencyCode":"USD","rateSchedule":"DM-RT01","startDate":"2020-01-01","isEligible":"false","assignmentLevel":"Customer Agreed","paTypeFlag":"RGLR","printIfZero":"Y","txnDailyRatingCrt":"DNRT","ignoreSw":"N","aggregateSw":"N","scheduleCode":"MONTHLY","priceCompDetails":{"priceCompId":"6068600091","priceCompDesc":"Basic","valueAmt":"12","displaySw":"true","rcMapId":"1705351562","tieredFlag":"FLAT","priceCompSequenceNo":"10"}}}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"modelId":"0028986982","dealId":"8402244329","entityType":"PERS","entityId":"8797366188","pricingAndCommitmentsDetails":{"entityDivision":"IND","entityIdentifierType":"COREG","entityType":"PERS","entityId":"8797366188","entityIdentifierValue":"Reg_BANK_82_EPER_001","pricingDetails":[{"txnDailyRatingCrt":"DNRT","priceCompDetails":{"priceCompId":"5417300006","valueAmt":"11","priceCompDesc":"FLAT","rcMapId":"1705351562","displaySw":"true","tieredFlag":"FLAT","priceCompSequenceNo":"10"},"paTypeFlag":"RGLR","priceItemDescription":"V2-Monthly Acct Serv Fee","aggregateSw":"Y","priceItemCode":"PI_022","priceCurrencyCode":"USD","priceAsgnId":"5410009203","pricingStatus":"PRPD","printIfZero":"Y","ignoreSw":"N","actionFlag":"OVRD","isEligible":"false","scheduleCode":"MONTHLY","rateSchedule":"DM-RT01","startDate":"2023-08-11","assignmentLevel":"Customer Price List"}]}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"dealId":"8402244329","modelId":"0028986982","entityId":"8797366188","entityType":"PERS","pricingAndCommitmentsDetails":{"entityId":"8797366188","entityType":"PERS","entityIdentifierValue":"Reg_BANK_82_EPER_001","entityIdentifierType":"COREG","entityDivision":"IND","pricingDetails":{"priceAsgnId":"5300014284","actionFlag":"OVRD","priceItemCode":"PI_022","priceItemDescription":"V2-Monthly Acct Serv Fee","pricingStatus":"PRPD","priceCurrencyCode":"USD","rateSchedule":"DM-RT01","startDate":"2023-08-11","isEligible":"false","assignmentLevel":"Customer Price List","paTypeFlag":"RGLR","printIfZero":"Y","txnDailyRatingCrt":"DNRT","ignoreSw":"N","aggregateSw":"Y","scheduleCode":"MONTHLY","priceCompDetails":{"priceCompId":"5417300006","priceCompDesc":"FLAT","valueAmt":"11","displaySw":"true","rcMapId":"1705351562","tieredFlag":"FLAT","priceCompSequenceNo":"10"}}}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"modelId":"0028986982","dealId":"8402244329","entityType":"PERS","entityId":"8797366188","pricingAndCommitmentsDetails":{"entityDivision":"IND","entityIdentifierType":"COREG","entityType":"PERS","entityId":"8797366188","entityIdentifierValue":"Reg_BANK_82_EPER_001","pricingDetails":[{"txnDailyRatingCrt":"DNRT","priceCompDetails":{"priceCompId":"5308600527","valueAmt":"10","priceCompDesc":"FLAT","rcMapId":"1705351562","displaySw":"true","tieredFlag":"FLAT","priceCompSequenceNo":"10"},"paTypeFlag":"RGLR","priceItemDescription":"V2-Monthly Acct Serv Fee","aggregateSw":"N","priceItemCode":"PI_022","priceCurrencyCode":"USD","priceAsgnId":"5300014284","pricingStatus":"PRPD","printIfZero":"Y","ignoreSw":"N","actionFlag":"OVRD","isEligible":"false","scheduleCode":"MONTHLY","rateSchedule":"DM-RT01","startDate":"2023-09-10","assignmentLevel":"Customer Agreed"}]}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"dealId":"8402244329","modelId":"0028986982","entityId":"8797366188","entityType":"PERS","pricingAndCommitmentsDetails":{"entityId":"8797366188","entityType":"PERS","entityIdentifierValue":"Reg_BANK_82_EPER_001","entityIdentifierType":"COREG","entityDivision":"IND","pricingDetails":{"priceAsgnId":"5300014285","actionFlag":"OVRD","priceItemCode":"PI_022","priceItemDescription":"V2-Monthly Acct Serv Fee","pricingStatus":"PRPD","priceCurrencyCode":"USD","rateSchedule":"DM-RT01","startDate":"2023-09-10","isEligible":"false","assignmentLevel":"Customer Agreed","paTypeFlag":"RGLR","printIfZero":"Y","txnDailyRatingCrt":"DNRT","ignoreSw":"N","aggregateSw":"N","scheduleCode":"MONTHLY","priceCompDetails":{"priceCompId":"5308600527","priceCompDesc":"FLAT","valueAmt":"10","displaySw":"true","rcMapId":"1705351562","tieredFlag":"FLAT","priceCompSequenceNo":"10"}}}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"modelId":"0028986982","dealId":"8402244329","entityType":"PERS","entityId":"8797366188","pricingAndCommitmentsDetails":{"entityDivision":"IND","entityIdentifierType":"COREG","entityType":"PERS","entityId":"8797366188","entityIdentifierValue":"Reg_BANK_82_EPER_001","pricingDetails":[{"txnDailyRatingCrt":"DNRT","priceCompDetails":[{"priceCompId":"5417400004","valueAmt":"11","priceCompDesc":"Price per transaction - Step Tier 1","rcMapId":"2567418376","displaySw":"true","tieredFlag":"STEP","priceCompTier":{"tierSeqNum":"10","upperLimit":"1000.00","lowerLimit":"0.00","priceCriteria":"NBRTRAN"},"priceCompSequenceNo":"100"},{"priceCompId":"5417400005","valueAmt":"12","priceCompDesc":"Price per transaction - Step Tier 2","rcMapId":"7769990702","displaySw":"true","tieredFlag":"STEP","priceCompTier":{"tierSeqNum":"10","upperLimit":"5000.00","lowerLimit":"1000.00","priceCriteria":"NBRTRAN"},"priceCompSequenceNo":"110"},{"priceCompId":"5417400006","valueAmt":"13","priceCompDesc":"Price per transaction - Step Tier 3","rcMapId":"4322456059","displaySw":"true","tieredFlag":"STEP","priceCompTier":{"tierSeqNum":"10","upperLimit":"999999999999.99","lowerLimit":"5000.00","priceCriteria":"NBRTRAN"},"priceCompSequenceNo":"120"}],"paTypeFlag":"RGLR","priceItemDescription":"V4-SEPA Transfers","aggregateSw":"Y","priceItemCode":"PI_024","priceCurrencyCode":"USD","priceAsgnId":"5410009241","pricingStatus":"PRPD","printIfZero":"Y","ignoreSw":"N","actionFlag":"OVRD","isEligible":"false","scheduleCode":"MONTHLY","rateSchedule":"DM-NBRST","startDate":"2023-08-11","assignmentLevel":"Customer Price List"}]}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"dealId":"8402244329","modelId":"0028986982","entityId":"8797366188","entityType":"PERS","pricingAndCommitmentsDetails":{"entityId":"8797366188","entityType":"PERS","entityIdentifierValue":"Reg_BANK_82_EPER_001","entityIdentifierType":"COREG","entityDivision":"IND","pricingDetails":{"priceAsgnId":"5300014286","actionFlag":"OVRD","priceItemCode":"PI_024","priceItemDescription":"V4-SEPA Transfers","pricingStatus":"PRPD","priceCurrencyCode":"USD","rateSchedule":"DM-NBRST","startDate":"2023-08-11","isEligible":"false","assignmentLevel":"Customer Price List","paTypeFlag":"RGLR","printIfZero":"Y","txnDailyRatingCrt":"DNRT","ignoreSw":"N","aggregateSw":"Y","scheduleCode":"MONTHLY","priceCompDetails":[{"priceCompTier":{"upperLimit":"1000.00","lowerLimit":"0.00","priceCriteria":"NBRTRAN","tierSeqNum":"10"},"priceCompId":"5417400004","priceCompDesc":"Price per transaction - Step Tier 1","valueAmt":"11","displaySw":"true","rcMapId":"2567418376","tieredFlag":"STEP","priceCompSequenceNo":"100"},{"priceCompTier":{"upperLimit":"5000.00","lowerLimit":"1000.00","priceCriteria":"NBRTRAN","tierSeqNum":"10"},"priceCompId":"5417400005","priceCompDesc":"Price per transaction - Step Tier 2","valueAmt":"12","displaySw":"true","rcMapId":"7769990702","tieredFlag":"STEP","priceCompSequenceNo":"110"},{"priceCompTier":{"upperLimit":"999999999999.99","lowerLimit":"5000.00","priceCriteria":"NBRTRAN","tierSeqNum":"10"},"priceCompId":"5417400006","priceCompDesc":"Price per transaction - Step Tier 3","valueAmt":"13","displaySw":"true","rcMapId":"4322456059","tieredFlag":"STEP","priceCompSequenceNo":"120"}]}}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"modelId":"0028986982","dealId":"8402244329","entityType":"PERS","entityId":"8797366188","pricingAndCommitmentsDetails":{"entityDivision":"IND","entityIdentifierType":"COREG","entityType":"PERS","entityId":"8797366188","entityIdentifierValue":"Reg_BANK_82_EPER_001","pricingDetails":[{"txnDailyRatingCrt":"DNRT","priceCompDetails":[{"priceCompId":"5308600529","valueAmt":"12","priceCompDesc":"Price per transaction - Step Tier 1","rcMapId":"2567418376","displaySw":"true","tieredFlag":"STEP","priceCompTier":{"tierSeqNum":"10","upperLimit":"1000.00","lowerLimit":"0.00","priceCriteria":"NBRTRAN"},"priceCompSequenceNo":"100"},{"priceCompId":"5308600530","valueAmt":"13","priceCompDesc":"Price per transaction - Step Tier 2","rcMapId":"7769990702","displaySw":"true","tieredFlag":"STEP","priceCompTier":{"tierSeqNum":"10","upperLimit":"5000.00","lowerLimit":"1000.00","priceCriteria":"NBRTRAN"},"priceCompSequenceNo":"110"},{"priceCompId":"5308600531","valueAmt":"14","priceCompDesc":"Price per transaction - Step Tier 3","rcMapId":"4322456059","displaySw":"true","tieredFlag":"STEP","priceCompTier":{"tierSeqNum":"10","upperLimit":"999999999999.99","lowerLimit":"5000.00","priceCriteria":"NBRTRAN"},"priceCompSequenceNo":"120"}],"paTypeFlag":"RGLR","priceItemDescription":"V4-SEPA Transfers","aggregateSw":"N","priceItemCode":"PI_024","priceCurrencyCode":"USD","priceAsgnId":"5300014286","pricingStatus":"PRPD","printIfZero":"Y","ignoreSw":"N","actionFlag":"OVRD","isEligible":"false","scheduleCode":"MONTHLY","rateSchedule":"DM-NBRST","startDate":"2023-09-10","assignmentLevel":"Customer Agreed"}]}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"dealId":"8402244329","modelId":"0028986982","entityId":"8797366188","entityType":"PERS","pricingAndCommitmentsDetails":{"entityId":"8797366188","entityType":"PERS","entityIdentifierValue":"Reg_BANK_82_EPER_001","entityIdentifierType":"COREG","entityDivision":"IND","pricingDetails":{"priceAsgnId":"5300014287","actionFlag":"OVRD","priceItemCode":"PI_024","priceItemDescription":"V4-SEPA Transfers","pricingStatus":"PRPD","priceCurrencyCode":"USD","rateSchedule":"DM-NBRST","startDate":"2023-09-10","isEligible":"false","assignmentLevel":"Customer Agreed","paTypeFlag":"RGLR","printIfZero":"Y","txnDailyRatingCrt":"DNRT","ignoreSw":"N","aggregateSw":"N","scheduleCode":"MONTHLY","priceCompDetails":[{"priceCompTier":{"upperLimit":"1000.00","lowerLimit":"0.00","priceCriteria":"NBRTRAN","tierSeqNum":"10"},"priceCompId":"5308600529","priceCompDesc":"Price per transaction - Step Tier 1","valueAmt":"12","displaySw":"true","rcMapId":"2567418376","tieredFlag":"STEP","priceCompSequenceNo":"100"},{"priceCompTier":{"upperLimit":"5000.00","lowerLimit":"1000.00","priceCriteria":"NBRTRAN","tierSeqNum":"10"},"priceCompId":"5308600530","priceCompDesc":"Price per transaction - Step Tier 2","valueAmt":"13","displaySw":"true","rcMapId":"7769990702","tieredFlag":"STEP","priceCompSequenceNo":"110"},{"priceCompTier":{"upperLimit":"999999999999.99","lowerLimit":"5000.00","priceCriteria":"NBRTRAN","tierSeqNum":"10"},"priceCompId":"5308600531","priceCompDesc":"Price per transaction - Step Tier 3","valueAmt":"14","displaySw":"true","rcMapId":"4322456059","tieredFlag":"STEP","priceCompSequenceNo":"120"}]}}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"modelId":"0028986982","dealId":"8402244329","entityType":"PERS","entityId":"8797366188","pricingAndCommitmentsDetails":{"entityDivision":"IND","entityIdentifierType":"COREG","entityType":"PERS","entityId":"8797366188","entityIdentifierValue":"Reg_BANK_82_EPER_001","pricingDetails":[{"txnDailyRatingCrt":"DNRT","priceCompDetails":[{"priceCompId":"5417400010","valueAmt":"11","priceCompDesc":"Threshold price per transaction","rcMapId":"1109655113","displaySw":"true","tieredFlag":"THRS","priceCompTier":{"tierSeqNum":"10","upperLimit":"1000.00","lowerLimit":"0.00","priceCriteria":"NBRTRAN"},"priceCompSequenceNo":"100"},{"priceCompId":"5417400011","valueAmt":"12","priceCompDesc":"Threshold price per transaction","rcMapId":"1109655113","displaySw":"true","tieredFlag":"THRS","priceCompTier":{"tierSeqNum":"10","upperLimit":"5000.00","lowerLimit":"1000.00","priceCriteria":"NBRTRAN"},"priceCompSequenceNo":"110"},{"priceCompId":"5417400012","valueAmt":"13","priceCompDesc":"Threshold price per transaction","rcMapId":"1109655113","displaySw":"true","tieredFlag":"THRS","priceCompTier":{"tierSeqNum":"10","upperLimit":"999999999999.99","lowerLimit":"5000.00","priceCriteria":"NBRTRAN"},"priceCompSequenceNo":"120"}],"paTypeFlag":"RGLR","priceItemDescription":"V5-Domestic Funds Transfer Fee","aggregateSw":"Y","priceItemCode":"PI_025","priceCurrencyCode":"USD","priceAsgnId":"5410009242","pricingStatus":"PRPD","printIfZero":"Y","ignoreSw":"N","actionFlag":"OVRD","isEligible":"false","scheduleCode":"MONTHLY","rateSchedule":"DM-NBRTH","startDate":"2023-08-11","assignmentLevel":"Customer Price List"}]}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"dealId":"8402244329","modelId":"0028986982","entityId":"8797366188","entityType":"PERS","pricingAndCommitmentsDetails":{"entityId":"8797366188","entityType":"PERS","entityIdentifierValue":"Reg_BANK_82_EPER_001","entityIdentifierType":"COREG","entityDivision":"IND","pricingDetails":{"priceAsgnId":"5300014288","actionFlag":"OVRD","priceItemCode":"PI_025","priceItemDescription":"V5-Domestic Funds Transfer Fee","pricingStatus":"PRPD","priceCurrencyCode":"USD","rateSchedule":"DM-NBRTH","startDate":"2023-08-11","isEligible":"false","assignmentLevel":"Customer Price List","paTypeFlag":"RGLR","printIfZero":"Y","txnDailyRatingCrt":"DNRT","ignoreSw":"N","aggregateSw":"Y","scheduleCode":"MONTHLY","priceCompDetails":[{"priceCompTier":{"upperLimit":"1000.00","lowerLimit":"0.00","priceCriteria":"NBRTRAN","tierSeqNum":"10"},"priceCompId":"5417400010","priceCompDesc":"Threshold price per transaction","valueAmt":"11","displaySw":"true","rcMapId":"1109655113","tieredFlag":"THRS","priceCompSequenceNo":"100"},{"priceCompTier":{"upperLimit":"5000.00","lowerLimit":"1000.00","priceCriteria":"NBRTRAN","tierSeqNum":"10"},"priceCompId":"5417400011","priceCompDesc":"Threshold price per transaction","valueAmt":"12","displaySw":"true","rcMapId":"1109655113","tieredFlag":"THRS","priceCompSequenceNo":"110"},{"priceCompTier":{"upperLimit":"999999999999.99","lowerLimit":"5000.00","priceCriteria":"NBRTRAN","tierSeqNum":"10"},"priceCompId":"5417400012","priceCompDesc":"Threshold price per transaction","valueAmt":"13","displaySw":"true","rcMapId":"1109655113","tieredFlag":"THRS","priceCompSequenceNo":"120"}]}}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"modelId":"0028986982","dealId":"8402244329","entityType":"PERS","entityId":"8797366188","pricingAndCommitmentsDetails":{"entityDivision":"IND","entityIdentifierType":"COREG","entityType":"PERS","entityId":"8797366188","entityIdentifierValue":"Reg_BANK_82_EPER_001","pricingDetails":[{"txnDailyRatingCrt":"DNRT","priceCompDetails":[{"priceCompId":"5308600535","valueAmt":"12","priceCompDesc":"Threshold price per transaction","rcMapId":"1109655113","displaySw":"true","tieredFlag":"THRS","priceCompTier":{"tierSeqNum":"10","upperLimit":"1000.00","lowerLimit":"0.00","priceCriteria":"NBRTRAN"},"priceCompSequenceNo":"100"},{"priceCompId":"5308600536","valueAmt":"13","priceCompDesc":"Threshold price per transaction","rcMapId":"1109655113","displaySw":"true","tieredFlag":"THRS","priceCompTier":{"tierSeqNum":"10","upperLimit":"5000.00","lowerLimit":"1000.00","priceCriteria":"NBRTRAN"},"priceCompSequenceNo":"110"},{"priceCompId":"5308600537","valueAmt":"14","priceCompDesc":"Threshold price per transaction","rcMapId":"1109655113","displaySw":"true","tieredFlag":"THRS","priceCompTier":{"tierSeqNum":"10","upperLimit":"999999999999.99","lowerLimit":"5000.00","priceCriteria":"NBRTRAN"},"priceCompSequenceNo":"120"}],"paTypeFlag":"RGLR","priceItemDescription":"V5-Domestic Funds Transfer Fee","aggregateSw":"N","priceItemCode":"PI_025","priceCurrencyCode":"USD","priceAsgnId":"5300014288","pricingStatus":"PRPD","printIfZero":"Y","ignoreSw":"N","actionFlag":"OVRD","isEligible":"false","scheduleCode":"MONTHLY","rateSchedule":"DM-NBRTH","startDate":"2023-09-10","assignmentLevel":"Customer Agreed"}]}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"dealId":"8402244329","modelId":"0028986982","entityId":"8797366188","entityType":"PERS","pricingAndCommitmentsDetails":{"entityId":"8797366188","entityType":"PERS","entityIdentifierValue":"Reg_BANK_82_EPER_001","entityIdentifierType":"COREG","entityDivision":"IND","pricingDetails":{"priceAsgnId":"5300014289","actionFlag":"OVRD","priceItemCode":"PI_025","priceItemDescription":"V5-Domestic Funds Transfer Fee","pricingStatus":"PRPD","priceCurrencyCode":"USD","rateSchedule":"DM-NBRTH","startDate":"2023-09-10","isEligible":"false","assignmentLevel":"Customer Agreed","paTypeFlag":"RGLR","printIfZero":"Y","txnDailyRatingCrt":"DNRT","ignoreSw":"N","aggregateSw":"N","scheduleCode":"MONTHLY","priceCompDetails":[{"priceCompTier":{"upperLimit":"1000.00","lowerLimit":"0.00","priceCriteria":"NBRTRAN","tierSeqNum":"10"},"priceCompId":"5308600535","priceCompDesc":"Threshold price per transaction","valueAmt":"12","displaySw":"true","rcMapId":"1109655113","tieredFlag":"THRS","priceCompSequenceNo":"100"},{"priceCompTier":{"upperLimit":"5000.00","lowerLimit":"1000.00","priceCriteria":"NBRTRAN","tierSeqNum":"10"},"priceCompId":"5308600536","priceCompDesc":"Threshold price per transaction","valueAmt":"13","displaySw":"true","rcMapId":"1109655113","tieredFlag":"THRS","priceCompSequenceNo":"110"},{"priceCompTier":{"upperLimit":"999999999999.99","lowerLimit":"5000.00","priceCriteria":"NBRTRAN","tierSeqNum":"10"},"priceCompId":"5308600537","priceCompDesc":"Threshold price per transaction","valueAmt":"14","displaySw":"true","rcMapId":"1109655113","tieredFlag":"THRS","priceCompSequenceNo":"120"}]}}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"modelId":"0028986982","dealId":"8402244329","entityType":"PERS","entityId":"8797366188","pricingAndCommitmentsDetails":{"entityDivision":"IND","entityIdentifierType":"COREG","entityType":"PERS","entityId":"8797366188","entityIdentifierValue":"Reg_BANK_82_EPER_001","pricingDetails":[{"txnDailyRatingCrt":"DNRT","priceCompDetails":{"priceCompId":"5417300044","valueAmt":"3","priceCompDesc":"FLAT","rcMapId":"1705351562","displaySw":"true","tieredFlag":"FLAT","priceCompSequenceNo":"10"},"parameterDetails":[{"parameterCode":"DM_CURRENCY","parameterValue":"INR"},{"parameterCode":"DM_TYPE","parameterValue":"BT"}],"paTypeFlag":"RGLR","priceItemDescription":"V8-Cheque Collections","aggregateSw":"Y","priceItemCode":"PI_028","priceCurrencyCode":"USD","priceAsgnId":"5410009212","pricingStatus":"PRPD","printIfZero":"Y","ignoreSw":"N","actionFlag":"OVRD","isEligible":"false","scheduleCode":"MONTHLY","rateSchedule":"DM-RT01","startDate":"2023-08-11","assignmentLevel":"Customer Price List"}]}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"dealId":"8402244329","modelId":"0028986982","entityId":"8797366188","entityType":"PERS","pricingAndCommitmentsDetails":{"entityId":"8797366188","entityType":"PERS","entityIdentifierValue":"Reg_BANK_82_EPER_001","entityIdentifierType":"COREG","entityDivision":"IND","pricingDetails":{"priceAsgnId":"5300014290","actionFlag":"OVRD","priceItemCode":"PI_028","priceItemDescription":"V8-Cheque Collections","pricingStatus":"PRPD","priceCurrencyCode":"USD","rateSchedule":"DM-RT01","startDate":"2023-08-11","isEligible":"false","assignmentLevel":"Customer Price List","paTypeFlag":"RGLR","printIfZero":"Y","parameterDetails":[{"parameterCode":"DM_CURRENCY","parameterValue":"INR"},{"parameterCode":"DM_TYPE","parameterValue":"BT"}],"txnDailyRatingCrt":"DNRT","ignoreSw":"N","aggregateSw":"Y","scheduleCode":"MONTHLY","priceCompDetails":{"priceCompId":"5417300044","priceCompDesc":"FLAT","valueAmt":"3","displaySw":"true","rcMapId":"1705351562","tieredFlag":"FLAT","priceCompSequenceNo":"10"}}}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"modelId":"0028986982","dealId":"8402244329","entityType":"PERS","entityId":"8797366188","pricingAndCommitmentsDetails":{"entityDivision":"IND","entityIdentifierType":"COREG","entityType":"PERS","entityId":"8797366188","entityIdentifierValue":"Reg_BANK_82_EPER_001","pricingDetails":[{"txnDailyRatingCrt":"DNRT","priceCompDetails":{"priceCompId":"5308600541","valueAmt":"2","priceCompDesc":"FLAT","rcMapId":"1705351562","displaySw":"true","tieredFlag":"FLAT","priceCompSequenceNo":"10"},"parameterDetails":[{"parameterCode":"DM_CURRENCY","parameterValue":"INR"},{"parameterCode":"DM_TYPE","parameterValue":"BT"}],"paTypeFlag":"RGLR","priceItemDescription":"V8-Cheque Collections","aggregateSw":"N","priceItemCode":"PI_028","priceCurrencyCode":"USD","priceAsgnId":"5300014290","pricingStatus":"PRPD","printIfZero":"Y","ignoreSw":"N","actionFlag":"OVRD","isEligible":"false","scheduleCode":"MONTHLY","rateSchedule":"DM-RT01","startDate":"2023-09-10","assignmentLevel":"Customer Agreed"}]}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"dealId":"8402244329","modelId":"0028986982","entityId":"8797366188","entityType":"PERS","pricingAndCommitmentsDetails":{"entityId":"8797366188","entityType":"PERS","entityIdentifierValue":"Reg_BANK_82_EPER_001","entityIdentifierType":"COREG","entityDivision":"IND","pricingDetails":{"priceAsgnId":"5300014291","actionFlag":"OVRD","priceItemCode":"PI_028","priceItemDescription":"V8-Cheque Collections","pricingStatus":"PRPD","priceCurrencyCode":"USD","rateSchedule":"DM-RT01","startDate":"2023-09-10","isEligible":"false","assignmentLevel":"Customer Agreed","paTypeFlag":"RGLR","printIfZero":"Y","parameterDetails":[{"parameterCode":"DM_CURRENCY","parameterValue":"INR"},{"parameterCode":"DM_TYPE","parameterValue":"BT"}],"txnDailyRatingCrt":"DNRT","ignoreSw":"N","aggregateSw":"N","scheduleCode":"MONTHLY","priceCompDetails":{"priceCompId":"5308600541","priceCompDesc":"FLAT","valueAmt":"2","displaySw":"true","rcMapId":"1705351562","tieredFlag":"FLAT","priceCompSequenceNo":"10"}}}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"modelId":"0028986982","dealId":"8402244329","entityType":"PERS","entityId":"8797366188","pricingAndCommitmentsDetails":{"entityDivision":"IND","entityIdentifierType":"COREG","entityType":"PERS","entityId":"8797366188","entityIdentifierValue":"Reg_BANK_82_EPER_001","pricingDetails":[{"txnDailyRatingCrt":"DNRT","priceCompDetails":[{"priceCompId":"5308600524","valueAmt":"12","priceCompDesc":"Price Per Transaction Step Tier 1","rcMapId":"2567418376","displaySw":"true","tieredFlag":"STEP","priceCompTier":{"tierSeqNum":"10","upperLimit":"1000.00","lowerLimit":"0.00","priceCriteria":"NBRTRAN"},"priceCompSequenceNo":"100"},{"priceCompId":"5308600525","valueAmt":"13","priceCompDesc":"Price Per Transaction Step Tier 2","rcMapId":"7769990702","displaySw":"true","tieredFlag":"STEP","priceCompTier":{"tierSeqNum":"10","upperLimit":"5000.00","lowerLimit":"1000.00","priceCriteria":"NBRTRAN"},"priceCompSequenceNo":"110"},{"priceCompId":"5308600526","valueAmt":"14","priceCompDesc":"Price Per Transaction Step Tier 3","rcMapId":"4322456059","displaySw":"true","tieredFlag":"STEP","priceCompTier":{"tierSeqNum":"10","upperLimit":"99999999.99","lowerLimit":"5000.00","priceCriteria":"NBRTRAN"},"priceCompSequenceNo":"120"}],"parameterDetails":[{"parameterCode":"DM_COUNTRY","parameterValue":"IND"},{"parameterCode":"DM_STATE","parameterValue":"KA"}],"paTypeFlag":"RGLR","priceItemDescription":"Price Item NPI_036","aggregateSw":"N","priceItemCode":"NPI_036","priceCurrencyCode":"USD","priceAsgnId":"5300014283","pricingStatus":"PRPD","printIfZero":"Y","ignoreSw":"N","actionFlag":"UPD","isEligible":"false","scheduleCode":"MONTHLY","rateSchedule":"DM-NBRST","startDate":"2023-08-11","assignmentLevel":"Customer Agreed"}]}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"dealId":"8402244329","modelId":"0028986982","entityId":"8797366188","entityType":"PERS","pricingAndCommitmentsDetails":{"entityId":"8797366188","entityType":"PERS","entityIdentifierValue":"Reg_BANK_82_EPER_001","entityIdentifierType":"COREG","entityDivision":"IND","pricingDetails":{"priceAsgnId":"5300014283","actionFlag":"UPD","priceItemCode":"NPI_036","priceItemDescription":"Price Item NPI_036","pricingStatus":"PRPD","priceCurrencyCode":"USD","rateSchedule":"DM-NBRST","startDate":"2023-08-11","isEligible":"false","assignmentLevel":"Customer Agreed","paTypeFlag":"RGLR","printIfZero":"Y","parameterDetails":[{"parameterCode":"DM_COUNTRY","parameterValue":"IND"},{"parameterCode":"DM_STATE","parameterValue":"KA"}],"txnDailyRatingCrt":"DNRT","ignoreSw":"N","aggregateSw":"N","scheduleCode":"MONTHLY","priceCompDetails":[{"priceCompTier":{"upperLimit":"1000.00","lowerLimit":"0.00","priceCriteria":"NBRTRAN","tierSeqNum":"10"},"priceCompId":"5308600524","priceCompDesc":"Price Per Transaction Step Tier 1","valueAmt":"12","displaySw":"true","rcMapId":"2567418376","tieredFlag":"STEP","priceCompSequenceNo":"100"},{"priceCompTier":{"upperLimit":"5000.00","lowerLimit":"1000.00","priceCriteria":"NBRTRAN","tierSeqNum":"10"},"priceCompId":"5308600525","priceCompDesc":"Price Per Transaction Step Tier 2","valueAmt":"13","displaySw":"true","rcMapId":"7769990702","tieredFlag":"STEP","priceCompSequenceNo":"110"},{"priceCompTier":{"upperLimit":"99999999.99","lowerLimit":"5000.00","priceCriteria":"NBRTRAN","tierSeqNum":"10"},"priceCompId":"5308600526","priceCompDesc":"Price Per Transaction Step Tier 3","valueAmt":"14","displaySw":"true","rcMapId":"4322456059","tieredFlag":"STEP","priceCompSequenceNo":"120"}]}}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"modelId":"0028986982","dealId":"8402244329","entityType":"PERS","entityId":"8797366188","pricingAndCommitmentsDetails":{"entityDivision":"IND","entityIdentifierType":"COREG","entityType":"PERS","entityId":"8797366188","entityIdentifierValue":"Reg_BANK_82_EPER_001","pricingDetails":[{"txnDailyRatingCrt":"DNRT","priceCompDetails":[{"priceCompId":"5308600524","valueAmt":"11","priceCompDesc":"Price Per Transaction Step Tier 1","rcMapId":"2567418376","displaySw":"true","tieredFlag":"STEP","priceCompTier":{"tierSeqNum":"10","upperLimit":"1000.00","lowerLimit":"0.00","priceCriteria":"NBRTRAN"},"priceCompSequenceNo":"100"},{"priceCompId":"5308600525","valueAmt":"12","priceCompDesc":"Price Per Transaction Step Tier 2","rcMapId":"7769990702","displaySw":"true","tieredFlag":"STEP","priceCompTier":{"tierSeqNum":"10","upperLimit":"5000.00","lowerLimit":"1000.00","priceCriteria":"NBRTRAN"},"priceCompSequenceNo":"110"},{"priceCompId":"5308600526","valueAmt":"13","priceCompDesc":"Price Per Transaction Step Tier 3","rcMapId":"4322456059","displaySw":"true","tieredFlag":"STEP","priceCompTier":{"tierSeqNum":"10","upperLimit":"99999999.99","lowerLimit":"5000.00","priceCriteria":"NBRTRAN"},"priceCompSequenceNo":"120"}],"parameterDetails":[{"parameterCode":"DM_COUNTRY","parameterValue":"IND"},{"parameterCode":"DM_STATE","parameterValue":"KA"}],"paTypeFlag":"RGLR","priceItemDescription":"Price Item NPI_036","aggregateSw":"Y","priceItemCode":"NPI_036","priceCurrencyCode":"USD","priceAsgnId":"5300014283","pricingStatus":"PRPD","printIfZero":"Y","ignoreSw":"N","actionFlag":"OVRD","isEligible":"false","scheduleCode":"MONTHLY","rateSchedule":"DM-NBRST","startDate":"2023-09-10","assignmentLevel":"Customer Agreed"}]}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"dealId":"8402244329","modelId":"0028986982","entityId":"8797366188","entityType":"PERS","pricingAndCommitmentsDetails":{"entityId":"8797366188","entityType":"PERS","entityIdentifierValue":"Reg_BANK_82_EPER_001","entityIdentifierType":"COREG","entityDivision":"IND","pricingDetails":{"priceAsgnId":"5300014292","actionFlag":"OVRD","priceItemCode":"NPI_036","priceItemDescription":"Price Item NPI_036","pricingStatus":"PRPD","priceCurrencyCode":"USD","rateSchedule":"DM-NBRST","startDate":"2023-09-10","isEligible":"false","assignmentLevel":"Customer Agreed","paTypeFlag":"RGLR","printIfZero":"Y","parameterDetails":[{"parameterCode":"DM_COUNTRY","parameterValue":"IND"},{"parameterCode":"DM_STATE","parameterValue":"KA"}],"txnDailyRatingCrt":"DNRT","ignoreSw":"N","aggregateSw":"Y","scheduleCode":"MONTHLY","priceCompDetails":[{"priceCompTier":{"upperLimit":"1000.00","lowerLimit":"0.00","priceCriteria":"NBRTRAN","tierSeqNum":"10"},"priceCompId":"5308600524","priceCompDesc":"Price Per Transaction Step Tier 1","valueAmt":"11","displaySw":"true","rcMapId":"2567418376","tieredFlag":"STEP","priceCompSequenceNo":"100"},{"priceCompTier":{"upperLimit":"5000.00","lowerLimit":"1000.00","priceCriteria":"NBRTRAN","tierSeqNum":"10"},"priceCompId":"5308600525","priceCompDesc":"Price Per Transaction Step Tier 2","valueAmt":"12","displaySw":"true","rcMapId":"7769990702","tieredFlag":"STEP","priceCompSequenceNo":"110"},{"priceCompTier":{"upperLimit":"99999999.99","lowerLimit":"5000.00","priceCriteria":"NBRTRAN","tierSeqNum":"10"},"priceCompId":"5308600526","priceCompDesc":"Price Per Transaction Step Tier 3","valueAmt":"13","displaySw":"true","rcMapId":"4322456059","tieredFlag":"STEP","priceCompSequenceNo":"120"}]}}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"modelId":"0028986982","dealId":"8402244329","entityType":"PERS","entityId":"8797366188","pricingAndCommitmentsDetails":{"entityDivision":"IND","entityIdentifierType":"COREG","entityType":"PERS","entityId":"8797366188","entityIdentifierValue":"Reg_BANK_82_EPER_001","pricingDetails":[{"txnDailyRatingCrt":"DNRT","priceCompDetails":[{"priceCompId":"5308600521","valueAmt":"32","priceCompDesc":"Threshold price per transaction1","rcMapId":"1109655113","displaySw":"true","tieredFlag":"THRS","priceCompTier":{"tierSeqNum":"10","upperLimit":"1000.00","lowerLimit":"0.00","priceCriteria":"NBRTRAN"},"priceCompSequenceNo":"100"},{"priceCompId":"5308600522","valueAmt":"33","priceCompDesc":"Threshold price per transaction 2","rcMapId":"1109655113","displaySw":"true","tieredFlag":"THRS","priceCompTier":{"tierSeqNum":"10","upperLimit":"5000.00","lowerLimit":"1000.00","priceCriteria":"NBRTRAN"},"priceCompSequenceNo":"110"},{"priceCompId":"5308600523","valueAmt":"34","priceCompDesc":"Threshold price per transaction 3","rcMapId":"1109655113","displaySw":"true","tieredFlag":"THRS","priceCompTier":{"tierSeqNum":"10","upperLimit":"99999999.99","lowerLimit":"5000.00","priceCriteria":"NBRTRAN"},"priceCompSequenceNo":"120"}],"parameterDetails":[{"parameterCode":"DM_COUNTRY","parameterValue":"IND"},{"parameterCode":"DM_STATE","parameterValue":"AP"}],"paTypeFlag":"RGLR","priceItemDescription":"Price Item NPI_036","aggregateSw":"N","priceItemCode":"NPI_036","priceCurrencyCode":"USD","priceAsgnId":"5300014282","pricingStatus":"PRPD","printIfZero":"Y","ignoreSw":"N","actionFlag":"UPD","isEligible":"false","scheduleCode":"MONTHLY","rateSchedule":"DM-NBRTH","startDate":"2023-08-11","assignmentLevel":"Customer Agreed"}]}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"dealId":"8402244329","modelId":"0028986982","entityId":"8797366188","entityType":"PERS","pricingAndCommitmentsDetails":{"entityId":"8797366188","entityType":"PERS","entityIdentifierValue":"Reg_BANK_82_EPER_001","entityIdentifierType":"COREG","entityDivision":"IND","pricingDetails":{"priceAsgnId":"5300014282","actionFlag":"UPD","priceItemCode":"NPI_036","priceItemDescription":"Price Item NPI_036","pricingStatus":"PRPD","priceCurrencyCode":"USD","rateSchedule":"DM-NBRTH","startDate":"2023-08-11","isEligible":"false","assignmentLevel":"Customer Agreed","paTypeFlag":"RGLR","printIfZero":"Y","parameterDetails":[{"parameterCode":"DM_COUNTRY","parameterValue":"IND"},{"parameterCode":"DM_STATE","parameterValue":"AP"}],"txnDailyRatingCrt":"DNRT","ignoreSw":"N","aggregateSw":"N","scheduleCode":"MONTHLY","priceCompDetails":[{"priceCompTier":{"upperLimit":"1000.00","lowerLimit":"0.00","priceCriteria":"NBRTRAN","tierSeqNum":"10"},"priceCompId":"5308600521","priceCompDesc":"Threshold price per transaction1","valueAmt":"32","displaySw":"true","rcMapId":"1109655113","tieredFlag":"THRS","priceCompSequenceNo":"100"},{"priceCompTier":{"upperLimit":"5000.00","lowerLimit":"1000.00","priceCriteria":"NBRTRAN","tierSeqNum":"10"},"priceCompId":"5308600522","priceCompDesc":"Threshold price per transaction 2","valueAmt":"33","displaySw":"true","rcMapId":"1109655113","tieredFlag":"THRS","priceCompSequenceNo":"110"},{"priceCompTier":{"upperLimit":"99999999.99","lowerLimit":"5000.00","priceCriteria":"NBRTRAN","tierSeqNum":"10"},"priceCompId":"5308600523","priceCompDesc":"Threshold price per transaction 3","valueAmt":"34","displaySw":"true","rcMapId":"1109655113","tieredFlag":"THRS","priceCompSequenceNo":"120"}]}}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"modelId":"0028986982","dealId":"8402244329","entityType":"PERS","entityId":"8797366188","pricingAndCommitmentsDetails":{"entityDivision":"IND","entityIdentifierType":"COREG","entityType":"PERS","entityId":"8797366188","entityIdentifierValue":"Reg_BANK_82_EPER_001","pricingDetails":[{"txnDailyRatingCrt":"DNRT","priceCompDetails":[{"priceCompId":"5308600521","valueAmt":"31","priceCompDesc":"Threshold price per transaction1","rcMapId":"1109655113","displaySw":"true","tieredFlag":"THRS","priceCompTier":{"tierSeqNum":"10","upperLimit":"1000.00","lowerLimit":"0.00","priceCriteria":"NBRTRAN"},"priceCompSequenceNo":"100"},{"priceCompId":"5308600522","valueAmt":"32","priceCompDesc":"Threshold price per transaction 2","rcMapId":"1109655113","displaySw":"true","tieredFlag":"THRS","priceCompTier":{"tierSeqNum":"10","upperLimit":"5000.00","lowerLimit":"1000.00","priceCriteria":"NBRTRAN"},"priceCompSequenceNo":"110"},{"priceCompId":"5308600523","valueAmt":"33","priceCompDesc":"Threshold price per transaction 3","rcMapId":"1109655113","displaySw":"true","tieredFlag":"THRS","priceCompTier":{"tierSeqNum":"10","upperLimit":"99999999.99","lowerLimit":"5000.00","priceCriteria":"NBRTRAN"},"priceCompSequenceNo":"120"}],"parameterDetails":[{"parameterCode":"DM_COUNTRY","parameterValue":"IND"},{"parameterCode":"DM_STATE","parameterValue":"AP"}],"paTypeFlag":"RGLR","priceItemDescription":"Price Item NPI_036","aggregateSw":"Y","priceItemCode":"NPI_036","priceCurrencyCode":"USD","priceAsgnId":"5300014282","pricingStatus":"PRPD","printIfZero":"Y","ignoreSw":"N","actionFlag":"OVRD","isEligible":"false","scheduleCode":"MONTHLY","rateSchedule":"DM-NBRTH","startDate":"2023-09-10","assignmentLevel":"Customer Agreed"}]}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"dealId":"8402244329","modelId":"0028986982","entityId":"8797366188","entityType":"PERS","pricingAndCommitmentsDetails":{"entityId":"8797366188","entityType":"PERS","entityIdentifierValue":"Reg_BANK_82_EPER_001","entityIdentifierType":"COREG","entityDivision":"IND","pricingDetails":{"priceAsgnId":"5300014293","actionFlag":"OVRD","priceItemCode":"NPI_036","priceItemDescription":"Price Item NPI_036","pricingStatus":"PRPD","priceCurrencyCode":"USD","rateSchedule":"DM-NBRTH","startDate":"2023-09-10","isEligible":"false","assignmentLevel":"Customer Agreed","paTypeFlag":"RGLR","printIfZero":"Y","parameterDetails":[{"parameterCode":"DM_COUNTRY","parameterValue":"IND"},{"parameterCode":"DM_STATE","parameterValue":"AP"}],"txnDailyRatingCrt":"DNRT","ignoreSw":"N","aggregateSw":"Y","scheduleCode":"MONTHLY","priceCompDetails":[{"priceCompTier":{"upperLimit":"1000.00","lowerLimit":"0.00","priceCriteria":"NBRTRAN","tierSeqNum":"10"},"priceCompId":"5308600521","priceCompDesc":"Threshold price per transaction1","valueAmt":"31","displaySw":"true","rcMapId":"1109655113","tieredFlag":"THRS","priceCompSequenceNo":"100"},{"priceCompTier":{"upperLimit":"5000.00","lowerLimit":"1000.00","priceCriteria":"NBRTRAN","tierSeqNum":"10"},"priceCompId":"5308600522","priceCompDesc":"Threshold price per transaction 2","valueAmt":"32","displaySw":"true","rcMapId":"1109655113","tieredFlag":"THRS","priceCompSequenceNo":"110"},{"priceCompTier":{"upperLimit":"99999999.99","lowerLimit":"5000.00","priceCriteria":"NBRTRAN","tierSeqNum":"10"},"priceCompId":"5308600523","priceCompDesc":"Threshold price per transaction 3","valueAmt":"33","displaySw":"true","rcMapId":"1109655113","tieredFlag":"THRS","priceCompSequenceNo":"120"}]}}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"modelId":"0028986982","dealId":"8402244329","entityType":"PERS","entityId":"8797366188","pricingAndCommitmentsDetails":{"entityDivision":"IND","entityIdentifierType":"COREG","entityType":"PERS","entityId":"8797366188","entityIdentifierValue":"Reg_BANK_82_EPER_001","pricingDetails":[{"txnDailyRatingCrt":"DNRT","priceCompDetails":{"priceCompId":"5417300002","valueAmt":"11","priceCompDesc":"FLAT","rcMapId":"1705351562","displaySw":"true","tieredFlag":"FLAT","priceCompSequenceNo":"10"},"paTypeFlag":"RGLR","priceItemDescription":"MT943_SWIFT_01","aggregateSw":"Y","priceItemCode":"PI_031","priceCurrencyCode":"USD","priceAsgnId":"5410009201","pricingStatus":"PRPD","printIfZero":"Y","ignoreSw":"N","actionFlag":"OVRD","isEligible":"false","scheduleCode":"MONTHLY","rateSchedule":"DM-RT01","startDate":"2023-08-11","assignmentLevel":"Customer Price List"}]}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"dealId":"8402244329","modelId":"0028986982","entityId":"8797366188","entityType":"PERS","pricingAndCommitmentsDetails":{"entityId":"8797366188","entityType":"PERS","entityIdentifierValue":"Reg_BANK_82_EPER_001","entityIdentifierType":"COREG","entityDivision":"IND","pricingDetails":{"priceAsgnId":"5300014294","actionFlag":"OVRD","priceItemCode":"PI_031","priceItemDescription":"MT943_SWIFT_01","pricingStatus":"PRPD","priceCurrencyCode":"USD","rateSchedule":"DM-RT01","startDate":"2023-08-11","isEligible":"false","assignmentLevel":"Customer Price List","paTypeFlag":"RGLR","printIfZero":"Y","txnDailyRatingCrt":"DNRT","ignoreSw":"N","aggregateSw":"Y","scheduleCode":"MONTHLY","priceCompDetails":{"priceCompId":"5417300002","priceCompDesc":"FLAT","valueAmt":"11","displaySw":"true","rcMapId":"1705351562","tieredFlag":"FLAT","priceCompSequenceNo":"10"}}}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"modelId":"0028986982","dealId":"8402244329","entityType":"PERS","entityId":"8797366188","pricingAndCommitmentsDetails":{"entityDivision":"IND","entityIdentifierType":"COREG","entityType":"PERS","entityId":"8797366188","entityIdentifierValue":"Reg_BANK_82_EPER_001","pricingDetails":[{"txnDailyRatingCrt":"DNRT","priceCompDetails":{"priceCompId":"5308600549","valueAmt":"12","priceCompDesc":"FLAT","rcMapId":"1705351562","displaySw":"true","tieredFlag":"FLAT","priceCompSequenceNo":"10"},"paTypeFlag":"RGLR","priceItemDescription":"MT943_SWIFT_01","aggregateSw":"N","priceItemCode":"PI_031","priceCurrencyCode":"USD","priceAsgnId":"5300014294","pricingStatus":"PRPD","printIfZero":"Y","ignoreSw":"N","actionFlag":"OVRD","isEligible":"false","scheduleCode":"MONTHLY","rateSchedule":"DM-RT01","startDate":"2023-09-10","assignmentLevel":"Customer Agreed"}]}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"dealId":"8402244329","modelId":"0028986982","entityId":"8797366188","entityType":"PERS","pricingAndCommitmentsDetails":{"entityId":"8797366188","entityType":"PERS","entityIdentifierValue":"Reg_BANK_82_EPER_001","entityIdentifierType":"COREG","entityDivision":"IND","pricingDetails":{"priceAsgnId":"5300014295","actionFlag":"OVRD","priceItemCode":"PI_031","priceItemDescription":"MT943_SWIFT_01","pricingStatus":"PRPD","priceCurrencyCode":"USD","rateSchedule":"DM-RT01","startDate":"2023-09-10","isEligible":"false","assignmentLevel":"Customer Agreed","paTypeFlag":"RGLR","printIfZero":"Y","txnDailyRatingCrt":"DNRT","ignoreSw":"N","aggregateSw":"N","scheduleCode":"MONTHLY","priceCompDetails":{"priceCompId":"5308600549","priceCompDesc":"FLAT","valueAmt":"12","displaySw":"true","rcMapId":"1705351562","tieredFlag":"FLAT","priceCompSequenceNo":"10"}}}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"modelId":"0028986982","dealId":"8402244329","entityType":"PERS","entityId":"8797366188","pricingAndCommitmentsDetails":{"entityDivision":"IND","entityIdentifierType":"COREG","entityType":"PERS","entityId":"8797366188","entityIdentifierValue":"Reg_BANK_82_EPER_001","pricingDetails":[{"txnDailyRatingCrt":"DNRT","priceCompDetails":{"priceCompId":"5417300038","valueAmt":"777","priceCompDesc":"Basic BK-NBR","rcMapId":"9384470053","displaySw":"true","tieredFlag":"FLAT","priceCompSequenceNo":"10"},"paTypeFlag":"RGLR","priceItemDescription":"V7-Direct Debit","aggregateSw":"Y","priceItemCode":"PI_027","priceCurrencyCode":"USD","priceAsgnId":"5410009209","pricingStatus":"PRPD","printIfZero":"Y","ignoreSw":"N","actionFlag":"OVRD","isEligible":"false","scheduleCode":"MONTHLY","rateSchedule":"DM-RT03","startDate":"2023-08-11","assignmentLevel":"Customer Price List"}]}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"dealId":"8402244329","modelId":"0028986982","entityId":"8797366188","entityType":"PERS","pricingAndCommitmentsDetails":{"entityId":"8797366188","entityType":"PERS","entityIdentifierValue":"Reg_BANK_82_EPER_001","entityIdentifierType":"COREG","entityDivision":"IND","pricingDetails":{"priceAsgnId":"5300014296","actionFlag":"OVRD","priceItemCode":"PI_027","priceItemDescription":"V7-Direct Debit","pricingStatus":"PRPD","priceCurrencyCode":"USD","rateSchedule":"DM-RT03","startDate":"2023-08-11","isEligible":"false","assignmentLevel":"Customer Price List","paTypeFlag":"RGLR","printIfZero":"Y","txnDailyRatingCrt":"DNRT","ignoreSw":"N","aggregateSw":"Y","scheduleCode":"MONTHLY","priceCompDetails":{"priceCompId":"5417300038","priceCompDesc":"Basic BK-NBR","valueAmt":"777","displaySw":"true","rcMapId":"9384470053","tieredFlag":"FLAT","priceCompSequenceNo":"10"}}}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"modelId":"0028986982","dealId":"8402244329","entityType":"PERS","entityId":"8797366188","pricingAndCommitmentsDetails":{"entityDivision":"IND","entityIdentifierType":"COREG","entityType":"PERS","entityId":"8797366188","entityIdentifierValue":"Reg_BANK_82_EPER_001","pricingDetails":[{"txnDailyRatingCrt":"DNRT","priceCompDetails":{"priceCompId":"5308600551","valueAmt":"775","priceCompDesc":"Basic BK-NBR","rcMapId":"9384470053","displaySw":"true","tieredFlag":"FLAT","priceCompSequenceNo":"10"},"paTypeFlag":"RGLR","priceItemDescription":"V7-Direct Debit","aggregateSw":"N","priceItemCode":"PI_027","priceCurrencyCode":"USD","priceAsgnId":"5300014296","pricingStatus":"PRPD","printIfZero":"Y","ignoreSw":"N","actionFlag":"OVRD","isEligible":"false","scheduleCode":"MONTHLY","rateSchedule":"DM-RT03","startDate":"2023-09-10","assignmentLevel":"Customer Agreed"}]}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"dealId":"8402244329","modelId":"0028986982","entityId":"8797366188","entityType":"PERS","pricingAndCommitmentsDetails":{"entityId":"8797366188","entityType":"PERS","entityIdentifierValue":"Reg_BANK_82_EPER_001","entityIdentifierType":"COREG","entityDivision":"IND","pricingDetails":{"priceAsgnId":"5300014297","actionFlag":"OVRD","priceItemCode":"PI_027","priceItemDescription":"V7-Direct Debit","pricingStatus":"PRPD","priceCurrencyCode":"USD","rateSchedule":"DM-RT03","startDate":"2023-09-10","isEligible":"false","assignmentLevel":"Customer Agreed","paTypeFlag":"RGLR","printIfZero":"Y","txnDailyRatingCrt":"DNRT","ignoreSw":"N","aggregateSw":"N","scheduleCode":"MONTHLY","priceCompDetails":{"priceCompId":"5308600551","priceCompDesc":"Basic BK-NBR","valueAmt":"775","displaySw":"true","rcMapId":"9384470053","tieredFlag":"FLAT","priceCompSequenceNo":"10"}}}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"modelId":"0028986982","dealId":"8402244329","entityType":"PERS","entityId":"8797366188","pricingAndCommitmentsDetails":{"entityDivision":"IND","entityIdentifierType":"COREG","entityType":"PERS","entityId":"8797366188","entityIdentifierValue":"Reg_BANK_82_EPER_001","pricingDetails":[{"txnDailyRatingCrt":"DNRT","priceCompDetails":{"priceCompId":"5417300004","valueAmt":"13","priceCompDesc":"FLAT","rcMapId":"1705351562","displaySw":"true","tieredFlag":"FLAT","priceCompSequenceNo":"10"},"paTypeFlag":"RGLR","priceItemDescription":"V1-Account Opening Fee","aggregateSw":"Y","priceItemCode":"PI_021","priceCurrencyCode":"USD","priceAsgnId":"5410009202","pricingStatus":"PRPD","printIfZero":"Y","ignoreSw":"N","actionFlag":"OVRD","isEligible":"false","scheduleCode":"MONTHLY","rateSchedule":"DM-RT01","startDate":"2023-08-11","assignmentLevel":"Customer Price List"}]}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"dealId":"8402244329","modelId":"0028986982","entityId":"8797366188","entityType":"PERS","pricingAndCommitmentsDetails":{"entityId":"8797366188","entityType":"PERS","entityIdentifierValue":"Reg_BANK_82_EPER_001","entityIdentifierType":"COREG","entityDivision":"IND","pricingDetails":{"priceAsgnId":"5300014298","actionFlag":"OVRD","priceItemCode":"PI_021","priceItemDescription":"V1-Account Opening Fee","pricingStatus":"PRPD","priceCurrencyCode":"USD","rateSchedule":"DM-RT01","startDate":"2023-08-11","isEligible":"false","assignmentLevel":"Customer Price List","paTypeFlag":"RGLR","printIfZero":"Y","txnDailyRatingCrt":"DNRT","ignoreSw":"N","aggregateSw":"Y","scheduleCode":"MONTHLY","priceCompDetails":{"priceCompId":"5417300004","priceCompDesc":"FLAT","valueAmt":"13","displaySw":"true","rcMapId":"1705351562","tieredFlag":"FLAT","priceCompSequenceNo":"10"}}}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"modelId":"0028986982","dealId":"8402244329","entityType":"PERS","entityId":"8797366188","pricingAndCommitmentsDetails":{"entityDivision":"IND","entityIdentifierType":"COREG","entityType":"PERS","entityId":"8797366188","entityIdentifierValue":"Reg_BANK_82_EPER_001","pricingDetails":[{"txnDailyRatingCrt":"DNRT","priceCompDetails":{"priceCompId":"5308600553","valueAmt":"12","priceCompDesc":"FLAT","rcMapId":"1705351562","displaySw":"true","tieredFlag":"FLAT","priceCompSequenceNo":"10"},"paTypeFlag":"RGLR","priceItemDescription":"V1-Account Opening Fee","aggregateSw":"N","priceItemCode":"PI_021","priceCurrencyCode":"USD","priceAsgnId":"5300014298","pricingStatus":"PRPD","printIfZero":"Y","ignoreSw":"N","actionFlag":"OVRD","isEligible":"false","scheduleCode":"MONTHLY","rateSchedule":"DM-RT01","startDate":"2023-09-10","assignmentLevel":"Customer Agreed"}]}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"dealId":"8402244329","modelId":"0028986982","entityId":"8797366188","entityType":"PERS","pricingAndCommitmentsDetails":{"entityId":"8797366188","entityType":"PERS","entityIdentifierValue":"Reg_BANK_82_EPER_001","entityIdentifierType":"COREG","entityDivision":"IND","pricingDetails":{"priceAsgnId":"5300014299","actionFlag":"OVRD","priceItemCode":"PI_021","priceItemDescription":"V1-Account Opening Fee","pricingStatus":"PRPD","priceCurrencyCode":"USD","rateSchedule":"DM-RT01","startDate":"2023-09-10","isEligible":"false","assignmentLevel":"Customer Agreed","paTypeFlag":"RGLR","printIfZero":"Y","txnDailyRatingCrt":"DNRT","ignoreSw":"N","aggregateSw":"N","scheduleCode":"MONTHLY","priceCompDetails":{"priceCompId":"5308600553","priceCompDesc":"FLAT","valueAmt":"12","displaySw":"true","rcMapId":"1705351562","tieredFlag":"FLAT","priceCompSequenceNo":"10"}}}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"modelId":"0028986982","dealId":"8402244329","entityType":"PERS","entityId":"8797366188","pricingAndCommitmentsDetails":{"entityDivision":"IND","entityIdentifierType":"COREG","entityType":"PERS","entityId":"8797366188","entityIdentifierValue":"Reg_BANK_82_EPER_001","pricingDetails":[{"txnDailyRatingCrt":"DNRT","priceCompDetails":{"priceCompId":"5308600519","valueAmt":"12","priceCompDesc":"Basic","rcMapId":"1705351562","displaySw":"true","tieredFlag":"FLAT","priceCompSequenceNo":"10"},"paTypeFlag":"RGLR","priceItemDescription":"Price Item NPI_024","aggregateSw":"N","priceItemCode":"NPI_024","priceCurrencyCode":"USD","priceAsgnId":"5300014280","pricingStatus":"RECM","printIfZero":"Y","ignoreSw":"N","actionFlag":"RECM","isEligible":"false","scheduleCode":"MONTHLY","rateSchedule":"DM-RT01","startDate":"2020-01-01","assignmentLevel":"Customer Agreed"}]}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"dealId":"8402244329","modelId":"0028986982","entityId":"8797366188","entityType":"PERS","pricingAndCommitmentsDetails":{"entityId":"8797366188","entityType":"PERS","entityIdentifierValue":"Reg_BANK_82_EPER_001","entityIdentifierType":"COREG","entityDivision":"IND","pricingDetails":{"priceAsgnId":"5300014300","actionFlag":"RECM","priceItemCode":"NPI_024","priceItemDescription":"Price Item NPI_024","pricingStatus":"RECM","priceCurrencyCode":"USD","rateSchedule":"DM-RT01","startDate":"2020-01-01","isEligible":"false","assignmentLevel":"Customer Agreed","paTypeFlag":"RGLR","printIfZero":"Y","txnDailyRatingCrt":"DNRT","ignoreSw":"N","aggregateSw":"N","scheduleCode":"MONTHLY","priceCompDetails":{"priceCompId":"5308600519","priceCompDesc":"Basic","valueAmt":"12","displaySw":"true","rcMapId":"1705351562","tieredFlag":"FLAT","priceCompSequenceNo":"10"}}}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"modelId":"0028986982","dealId":"8402244329","entityType":"PERS","entityId":"8797366188","pricingAndCommitmentsDetails":{"entityDivision":"IND","entityIdentifierType":"COREG","entityType":"PERS","entityId":"8797366188","entityIdentifierValue":"Reg_BANK_82_EPER_001","pricingDetails":[{"txnDailyRatingCrt":"DNRT","priceCompDetails":{"priceCompId":"5308600519","valueAmt":"12","priceCompDesc":"Basic","rcMapId":"1705351562","displaySw":"true","tieredFlag":"FLAT","priceCompSequenceNo":"10"},"paTypeFlag":"RGLR","priceItemDescription":"Price Item NPI_024","aggregateSw":"N","priceItemCode":"NPI_024","priceCurrencyCode":"USD","priceAsgnId":"5300014280","pricingStatus":"PRPD","printIfZero":"Y","ignoreSw":"N","actionFlag":"UPD","isEligible":"false","scheduleCode":"MONTHLY","rateSchedule":"DM-RT01","startDate":"2020-01-01","assignmentLevel":"Customer Agreed"}]}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"dealId":"8402244329","modelId":"0028986982","entityId":"8797366188","entityType":"PERS","pricingAndCommitmentsDetails":{"entityId":"8797366188","entityType":"PERS","entityIdentifierValue":"Reg_BANK_82_EPER_001","entityIdentifierType":"COREG","entityDivision":"IND","pricingDetails":{"priceAsgnId":"5300014280","actionFlag":"UPD","priceItemCode":"NPI_024","priceItemDescription":"Price Item NPI_024","pricingStatus":"PRPD","priceCurrencyCode":"USD","rateSchedule":"DM-RT01","startDate":"2020-01-01","isEligible":"false","assignmentLevel":"Customer Agreed","paTypeFlag":"RGLR","printIfZero":"Y","txnDailyRatingCrt":"DNRT","ignoreSw":"N","aggregateSw":"N","scheduleCode":"MONTHLY","priceCompDetails":{"priceCompId":"5308600519","priceCompDesc":"Basic","valueAmt":"12","displaySw":"true","rcMapId":"1705351562","tieredFlag":"FLAT","priceCompSequenceNo":"10"}}}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"modelId":"3488649738","dealId":"4538544755","entityType":"PERS","entityId":"8797366188","pricingAndCommitmentsDetails":{"entityDivision":"IND","entityIdentifierType":"COREG","entityType":"PERS","entityId":"8797366188","entityIdentifierValue":"Reg_BANK_82_EPER_001","pricingDetails":[{"txnDailyRatingCrt":"DNRT","priceCompDetails":{"priceCompId":"5417300006","valueAmt":"11","priceCompDesc":"FLAT","rcMapId":"1705351562","displaySw":"true","tieredFlag":"FLAT","priceCompSequenceNo":"10"},"paTypeFlag":"RGLR","priceItemDescription":"V2-Monthly Acct Serv Fee","aggregateSw":"Y","priceItemCode":"PI_022","priceCurrencyCode":"USD","priceAsgnId":"5410009203","pricingStatus":"PRPD","printIfZero":"Y","ignoreSw":"N","actionFlag":"OVRD","isEligible":"false","scheduleCode":"MONTHLY","rateSchedule":"DM-RT01","startDate":"2023-08-12","assignmentLevel":"Customer Price List"}]}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"dealId":"4538544755","modelId":"3488649738","entityId":"8797366188","entityType":"PERS","pricingAndCommitmentsDetails":{"entityId":"8797366188","entityType":"PERS","entityIdentifierValue":"Reg_BANK_82_EPER_001","entityIdentifierType":"COREG","entityDivision":"IND","pricingDetails":{"priceAsgnId":"7650014576","actionFlag":"OVRD","priceItemCode":"PI_022","priceItemDescription":"V2-Monthly Acct Serv Fee","pricingStatus":"PRPD","priceCurrencyCode":"USD","rateSchedule":"DM-RT01","startDate":"2023-08-12","isEligible":"false","assignmentLevel":"Customer Price List","paTypeFlag":"RGLR","printIfZero":"Y","txnDailyRatingCrt":"DNRT","ignoreSw":"N","aggregateSw":"Y","scheduleCode":"MONTHLY","priceCompDetails":{"priceCompId":"5417300006","priceCompDesc":"FLAT","valueAmt":"11","displaySw":"true","rcMapId":"1705351562","tieredFlag":"FLAT","priceCompSequenceNo":"10"}}}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"modelId":"3488649738","dealId":"4538544755","entityType":"PERS","entityId":"8797366188","pricingAndCommitmentsDetails":{"entityDivision":"IND","entityIdentifierType":"COREG","entityType":"PERS","entityId":"8797366188","entityIdentifierValue":"Reg_BANK_82_EPER_001","pricingDetails":[{"txnDailyRatingCrt":"DNRT","priceCompDetails":{"priceCompId":"7658601058","valueAmt":"10","priceCompDesc":"FLAT","rcMapId":"1705351562","displaySw":"true","tieredFlag":"FLAT","priceCompSequenceNo":"10"},"paTypeFlag":"RGLR","priceItemDescription":"V2-Monthly Acct Serv Fee","aggregateSw":"N","priceItemCode":"PI_022","priceCurrencyCode":"USD","priceAsgnId":"7650014576","pricingStatus":"PRPD","printIfZero":"Y","ignoreSw":"N","actionFlag":"OVRD","isEligible":"false","scheduleCode":"MONTHLY","rateSchedule":"DM-RT01","startDate":"2023-09-11","assignmentLevel":"Customer Agreed"}]}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"dealId":"4538544755","modelId":"3488649738","entityId":"8797366188","entityType":"PERS","pricingAndCommitmentsDetails":{"entityId":"8797366188","entityType":"PERS","entityIdentifierValue":"Reg_BANK_82_EPER_001","entityIdentifierType":"COREG","entityDivision":"IND","pricingDetails":{"priceAsgnId":"7650014577","actionFlag":"OVRD","priceItemCode":"PI_022","priceItemDescription":"V2-Monthly Acct Serv Fee","pricingStatus":"PRPD","priceCurrencyCode":"USD","rateSchedule":"DM-RT01","startDate":"2023-09-11","isEligible":"false","assignmentLevel":"Customer Agreed","paTypeFlag":"RGLR","printIfZero":"Y","txnDailyRatingCrt":"DNRT","ignoreSw":"N","aggregateSw":"N","scheduleCode":"MONTHLY","priceCompDetails":{"priceCompId":"7658601058","priceCompDesc":"FLAT","valueAmt":"10","displaySw":"true","rcMapId":"1705351562","tieredFlag":"FLAT","priceCompSequenceNo":"10"}}}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"modelId":"3488649738","dealId":"4538544755","entityType":"PERS","entityId":"8797366188","pricingAndCommitmentsDetails":{"entityDivision":"IND","entityIdentifierType":"COREG","entityType":"PERS","entityId":"8797366188","entityIdentifierValue":"Reg_BANK_82_EPER_001","pricingDetails":[{"txnDailyRatingCrt":"DNRT","priceCompDetails":[{"priceCompId":"5417400004","valueAmt":"11","priceCompDesc":"Price per transaction - Step Tier 1","rcMapId":"2567418376","displaySw":"true","tieredFlag":"STEP","priceCompTier":{"tierSeqNum":"10","upperLimit":"1000.00","lowerLimit":"0.00","priceCriteria":"NBRTRAN"},"priceCompSequenceNo":"100"},{"priceCompId":"5417400005","valueAmt":"12","priceCompDesc":"Price per transaction - Step Tier 2","rcMapId":"7769990702","displaySw":"true","tieredFlag":"STEP","priceCompTier":{"tierSeqNum":"10","upperLimit":"5000.00","lowerLimit":"1000.00","priceCriteria":"NBRTRAN"},"priceCompSequenceNo":"110"},{"priceCompId":"5417400006","valueAmt":"13","priceCompDesc":"Price per transaction - Step Tier 3","rcMapId":"4322456059","displaySw":"true","tieredFlag":"STEP","priceCompTier":{"tierSeqNum":"10","upperLimit":"999999999999.99","lowerLimit":"5000.00","priceCriteria":"NBRTRAN"},"priceCompSequenceNo":"120"}],"paTypeFlag":"RGLR","priceItemDescription":"V4-SEPA Transfers","aggregateSw":"Y","priceItemCode":"PI_024","priceCurrencyCode":"USD","priceAsgnId":"5410009241","pricingStatus":"PRPD","printIfZero":"Y","ignoreSw":"N","actionFlag":"OVRD","isEligible":"false","scheduleCode":"MONTHLY","rateSchedule":"DM-NBRST","startDate":"2023-08-12","assignmentLevel":"Customer Price List"}]}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"dealId":"4538544755","modelId":"3488649738","entityId":"8797366188","entityType":"PERS","pricingAndCommitmentsDetails":{"entityId":"8797366188","entityType":"PERS","entityIdentifierValue":"Reg_BANK_82_EPER_001","entityIdentifierType":"COREG","entityDivision":"IND","pricingDetails":{"priceAsgnId":"7650014578","actionFlag":"OVRD","priceItemCode":"PI_024","priceItemDescription":"V4-SEPA Transfers","pricingStatus":"PRPD","priceCurrencyCode":"USD","rateSchedule":"DM-NBRST","startDate":"2023-08-12","isEligible":"false","assignmentLevel":"Customer Price List","paTypeFlag":"RGLR","printIfZero":"Y","txnDailyRatingCrt":"DNRT","ignoreSw":"N","aggregateSw":"Y","scheduleCode":"MONTHLY","priceCompDetails":[{"priceCompTier":{"upperLimit":"1000.00","lowerLimit":"0.00","priceCriteria":"NBRTRAN","tierSeqNum":"10"},"priceCompId":"5417400004","priceCompDesc":"Price per transaction - Step Tier 1","valueAmt":"11","displaySw":"true","rcMapId":"2567418376","tieredFlag":"STEP","priceCompSequenceNo":"100"},{"priceCompTier":{"upperLimit":"5000.00","lowerLimit":"1000.00","priceCriteria":"NBRTRAN","tierSeqNum":"10"},"priceCompId":"5417400005","priceCompDesc":"Price per transaction - Step Tier 2","valueAmt":"12","displaySw":"true","rcMapId":"7769990702","tieredFlag":"STEP","priceCompSequenceNo":"110"},{"priceCompTier":{"upperLimit":"999999999999.99","lowerLimit":"5000.00","priceCriteria":"NBRTRAN","tierSeqNum":"10"},"priceCompId":"5417400006","priceCompDesc":"Price per transaction - Step Tier 3","valueAmt":"13","displaySw":"true","rcMapId":"4322456059","tieredFlag":"STEP","priceCompSequenceNo":"120"}]}}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"modelId":"3488649738","dealId":"4538544755","entityType":"PERS","entityId":"8797366188","pricingAndCommitmentsDetails":{"entityDivision":"IND","entityIdentifierType":"COREG","entityType":"PERS","entityId":"8797366188","entityIdentifierValue":"Reg_BANK_82_EPER_001","pricingDetails":[{"txnDailyRatingCrt":"DNRT","priceCompDetails":[{"priceCompId":"7658601060","valueAmt":"12","priceCompDesc":"Price per transaction - Step Tier 1","rcMapId":"2567418376","displaySw":"true","tieredFlag":"STEP","priceCompTier":{"tierSeqNum":"10","upperLimit":"1000.00","lowerLimit":"0.00","priceCriteria":"NBRTRAN"},"priceCompSequenceNo":"100"},{"priceCompId":"7658601061","valueAmt":"13","priceCompDesc":"Price per transaction - Step Tier 2","rcMapId":"7769990702","displaySw":"true","tieredFlag":"STEP","priceCompTier":{"tierSeqNum":"10","upperLimit":"5000.00","lowerLimit":"1000.00","priceCriteria":"NBRTRAN"},"priceCompSequenceNo":"110"},{"priceCompId":"7658601062","valueAmt":"14","priceCompDesc":"Price per transaction - Step Tier 3","rcMapId":"4322456059","displaySw":"true","tieredFlag":"STEP","priceCompTier":{"tierSeqNum":"10","upperLimit":"999999999999.99","lowerLimit":"5000.00","priceCriteria":"NBRTRAN"},"priceCompSequenceNo":"120"}],"paTypeFlag":"RGLR","priceItemDescription":"V4-SEPA Transfers","aggregateSw":"N","priceItemCode":"PI_024","priceCurrencyCode":"USD","priceAsgnId":"7650014578","pricingStatus":"PRPD","printIfZero":"Y","ignoreSw":"N","actionFlag":"OVRD","isEligible":"false","scheduleCode":"MONTHLY","rateSchedule":"DM-NBRST","startDate":"2023-09-11","assignmentLevel":"Customer Agreed"}]}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"dealId":"4538544755","modelId":"3488649738","entityId":"8797366188","entityType":"PERS","pricingAndCommitmentsDetails":{"entityId":"8797366188","entityType":"PERS","entityIdentifierValue":"Reg_BANK_82_EPER_001","entityIdentifierType":"COREG","entityDivision":"IND","pricingDetails":{"priceAsgnId":"7650014579","actionFlag":"OVRD","priceItemCode":"PI_024","priceItemDescription":"V4-SEPA Transfers","pricingStatus":"PRPD","priceCurrencyCode":"USD","rateSchedule":"DM-NBRST","startDate":"2023-09-11","isEligible":"false","assignmentLevel":"Customer Agreed","paTypeFlag":"RGLR","printIfZero":"Y","txnDailyRatingCrt":"DNRT","ignoreSw":"N","aggregateSw":"N","scheduleCode":"MONTHLY","priceCompDetails":[{"priceCompTier":{"upperLimit":"1000.00","lowerLimit":"0.00","priceCriteria":"NBRTRAN","tierSeqNum":"10"},"priceCompId":"7658601060","priceCompDesc":"Price per transaction - Step Tier 1","valueAmt":"12","displaySw":"true","rcMapId":"2567418376","tieredFlag":"STEP","priceCompSequenceNo":"100"},{"priceCompTier":{"upperLimit":"5000.00","lowerLimit":"1000.00","priceCriteria":"NBRTRAN","tierSeqNum":"10"},"priceCompId":"7658601061","priceCompDesc":"Price per transaction - Step Tier 2","valueAmt":"13","displaySw":"true","rcMapId":"7769990702","tieredFlag":"STEP","priceCompSequenceNo":"110"},{"priceCompTier":{"upperLimit":"999999999999.99","lowerLimit":"5000.00","priceCriteria":"NBRTRAN","tierSeqNum":"10"},"priceCompId":"7658601062","priceCompDesc":"Price per transaction - Step Tier 3","valueAmt":"14","displaySw":"true","rcMapId":"4322456059","tieredFlag":"STEP","priceCompSequenceNo":"120"}]}}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"modelId":"3488649738","dealId":"4538544755","entityType":"PERS","entityId":"8797366188","pricingAndCommitmentsDetails":{"entityDivision":"IND","entityIdentifierType":"COREG","entityType":"PERS","entityId":"8797366188","entityIdentifierValue":"Reg_BANK_82_EPER_001","pricingDetails":[{"txnDailyRatingCrt":"DNRT","priceCompDetails":[{"priceCompId":"5417400010","valueAmt":"11","priceCompDesc":"Threshold price per transaction","rcMapId":"1109655113","displaySw":"true","tieredFlag":"THRS","priceCompTier":{"tierSeqNum":"10","upperLimit":"1000.00","lowerLimit":"0.00","priceCriteria":"NBRTRAN"},"priceCompSequenceNo":"100"},{"priceCompId":"5417400011","valueAmt":"12","priceCompDesc":"Threshold price per transaction","rcMapId":"1109655113","displaySw":"true","tieredFlag":"THRS","priceCompTier":{"tierSeqNum":"10","upperLimit":"5000.00","lowerLimit":"1000.00","priceCriteria":"NBRTRAN"},"priceCompSequenceNo":"110"},{"priceCompId":"5417400012","valueAmt":"13","priceCompDesc":"Threshold price per transaction","rcMapId":"1109655113","displaySw":"true","tieredFlag":"THRS","priceCompTier":{"tierSeqNum":"10","upperLimit":"999999999999.99","lowerLimit":"5000.00","priceCriteria":"NBRTRAN"},"priceCompSequenceNo":"120"}],"paTypeFlag":"RGLR","priceItemDescription":"V5-Domestic Funds Transfer Fee","aggregateSw":"Y","priceItemCode":"PI_025","priceCurrencyCode":"USD","priceAsgnId":"5410009242","pricingStatus":"PRPD","printIfZero":"Y","ignoreSw":"N","actionFlag":"OVRD","isEligible":"false","scheduleCode":"MONTHLY","rateSchedule":"DM-NBRTH","startDate":"2023-08-12","assignmentLevel":"Customer Price List"}]}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"dealId":"4538544755","modelId":"3488649738","entityId":"8797366188","entityType":"PERS","pricingAndCommitmentsDetails":{"entityId":"8797366188","entityType":"PERS","entityIdentifierValue":"Reg_BANK_82_EPER_001","entityIdentifierType":"COREG","entityDivision":"IND","pricingDetails":{"priceAsgnId":"7650014580","actionFlag":"OVRD","priceItemCode":"PI_025","priceItemDescription":"V5-Domestic Funds Transfer Fee","pricingStatus":"PRPD","priceCurrencyCode":"USD","rateSchedule":"DM-NBRTH","startDate":"2023-08-12","isEligible":"false","assignmentLevel":"Customer Price List","paTypeFlag":"RGLR","printIfZero":"Y","txnDailyRatingCrt":"DNRT","ignoreSw":"N","aggregateSw":"Y","scheduleCode":"MONTHLY","priceCompDetails":[{"priceCompTier":{"upperLimit":"1000.00","lowerLimit":"0.00","priceCriteria":"NBRTRAN","tierSeqNum":"10"},"priceCompId":"5417400010","priceCompDesc":"Threshold price per transaction","valueAmt":"11","displaySw":"true","rcMapId":"1109655113","tieredFlag":"THRS","priceCompSequenceNo":"100"},{"priceCompTier":{"upperLimit":"5000.00","lowerLimit":"1000.00","priceCriteria":"NBRTRAN","tierSeqNum":"10"},"priceCompId":"5417400011","priceCompDesc":"Threshold price per transaction","valueAmt":"12","displaySw":"true","rcMapId":"1109655113","tieredFlag":"THRS","priceCompSequenceNo":"110"},{"priceCompTier":{"upperLimit":"999999999999.99","lowerLimit":"5000.00","priceCriteria":"NBRTRAN","tierSeqNum":"10"},"priceCompId":"5417400012","priceCompDesc":"Threshold price per transaction","valueAmt":"13","displaySw":"true","rcMapId":"1109655113","tieredFlag":"THRS","priceCompSequenceNo":"120"}]}}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"modelId":"3488649738","dealId":"4538544755","entityType":"PERS","entityId":"8797366188","pricingAndCommitmentsDetails":{"entityDivision":"IND","entityIdentifierType":"COREG","entityType":"PERS","entityId":"8797366188","entityIdentifierValue":"Reg_BANK_82_EPER_001","pricingDetails":[{"txnDailyRatingCrt":"DNRT","priceCompDetails":[{"priceCompId":"7658601066","valueAmt":"12","priceCompDesc":"Threshold price per transaction","rcMapId":"1109655113","displaySw":"true","tieredFlag":"THRS","priceCompTier":{"tierSeqNum":"10","upperLimit":"1000.00","lowerLimit":"0.00","priceCriteria":"NBRTRAN"},"priceCompSequenceNo":"100"},{"priceCompId":"7658601067","valueAmt":"13","priceCompDesc":"Threshold price per transaction","rcMapId":"1109655113","displaySw":"true","tieredFlag":"THRS","priceCompTier":{"tierSeqNum":"10","upperLimit":"5000.00","lowerLimit":"1000.00","priceCriteria":"NBRTRAN"},"priceCompSequenceNo":"110"},{"priceCompId":"7658601068","valueAmt":"14","priceCompDesc":"Threshold price per transaction","rcMapId":"1109655113","displaySw":"true","tieredFlag":"THRS","priceCompTier":{"tierSeqNum":"10","upperLimit":"999999999999.99","lowerLimit":"5000.00","priceCriteria":"NBRTRAN"},"priceCompSequenceNo":"120"}],"paTypeFlag":"RGLR","priceItemDescription":"V5-Domestic Funds Transfer Fee","aggregateSw":"N","priceItemCode":"PI_025","priceCurrencyCode":"USD","priceAsgnId":"7650014580","pricingStatus":"PRPD","printIfZero":"Y","ignoreSw":"N","actionFlag":"OVRD","isEligible":"false","scheduleCode":"MONTHLY","rateSchedule":"DM-NBRTH","startDate":"2023-09-11","assignmentLevel":"Customer Agreed"}]}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"dealId":"4538544755","modelId":"3488649738","entityId":"8797366188","entityType":"PERS","pricingAndCommitmentsDetails":{"entityId":"8797366188","entityType":"PERS","entityIdentifierValue":"Reg_BANK_82_EPER_001","entityIdentifierType":"COREG","entityDivision":"IND","pricingDetails":{"priceAsgnId":"7650014581","actionFlag":"OVRD","priceItemCode":"PI_025","priceItemDescription":"V5-Domestic Funds Transfer Fee","pricingStatus":"PRPD","priceCurrencyCode":"USD","rateSchedule":"DM-NBRTH","startDate":"2023-09-11","isEligible":"false","assignmentLevel":"Customer Agreed","paTypeFlag":"RGLR","printIfZero":"Y","txnDailyRatingCrt":"DNRT","ignoreSw":"N","aggregateSw":"N","scheduleCode":"MONTHLY","priceCompDetails":[{"priceCompTier":{"upperLimit":"1000.00","lowerLimit":"0.00","priceCriteria":"NBRTRAN","tierSeqNum":"10"},"priceCompId":"7658601066","priceCompDesc":"Threshold price per transaction","valueAmt":"12","displaySw":"true","rcMapId":"1109655113","tieredFlag":"THRS","priceCompSequenceNo":"100"},{"priceCompTier":{"upperLimit":"5000.00","lowerLimit":"1000.00","priceCriteria":"NBRTRAN","tierSeqNum":"10"},"priceCompId":"7658601067","priceCompDesc":"Threshold price per transaction","valueAmt":"13","displaySw":"true","rcMapId":"1109655113","tieredFlag":"THRS","priceCompSequenceNo":"110"},{"priceCompTier":{"upperLimit":"999999999999.99","lowerLimit":"5000.00","priceCriteria":"NBRTRAN","tierSeqNum":"10"},"priceCompId":"7658601068","priceCompDesc":"Threshold price per transaction","valueAmt":"14","displaySw":"true","rcMapId":"1109655113","tieredFlag":"THRS","priceCompSequenceNo":"120"}]}}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"modelId":"3488649738","dealId":"4538544755","entityType":"PERS","entityId":"8797366188","pricingAndCommitmentsDetails":{"entityDivision":"IND","entityIdentifierType":"COREG","entityType":"PERS","entityId":"8797366188","entityIdentifierValue":"Reg_BANK_82_EPER_001","pricingDetails":[{"txnDailyRatingCrt":"DNRT","priceCompDetails":{"priceCompId":"5417300044","valueAmt":"3","priceCompDesc":"FLAT","rcMapId":"1705351562","displaySw":"true","tieredFlag":"FLAT","priceCompSequenceNo":"10"},"parameterDetails":[{"parameterCode":"DM_CURRENCY","parameterValue":"INR"},{"parameterCode":"DM_TYPE","parameterValue":"BT"}],"paTypeFlag":"RGLR","priceItemDescription":"V8-Cheque Collections","aggregateSw":"Y","priceItemCode":"PI_028","priceCurrencyCode":"USD","priceAsgnId":"5410009212","pricingStatus":"PRPD","printIfZero":"Y","ignoreSw":"N","actionFlag":"OVRD","isEligible":"false","scheduleCode":"MONTHLY","rateSchedule":"DM-RT01","startDate":"2023-08-12","assignmentLevel":"Customer Price List"}]}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"dealId":"4538544755","modelId":"3488649738","entityId":"8797366188","entityType":"PERS","pricingAndCommitmentsDetails":{"entityId":"8797366188","entityType":"PERS","entityIdentifierValue":"Reg_BANK_82_EPER_001","entityIdentifierType":"COREG","entityDivision":"IND","pricingDetails":{"priceAsgnId":"7650014582","actionFlag":"OVRD","priceItemCode":"PI_028","priceItemDescription":"V8-Cheque Collections","pricingStatus":"PRPD","priceCurrencyCode":"USD","rateSchedule":"DM-RT01","startDate":"2023-08-12","isEligible":"false","assignmentLevel":"Customer Price List","paTypeFlag":"RGLR","printIfZero":"Y","parameterDetails":[{"parameterCode":"DM_CURRENCY","parameterValue":"INR"},{"parameterCode":"DM_TYPE","parameterValue":"BT"}],"txnDailyRatingCrt":"DNRT","ignoreSw":"N","aggregateSw":"Y","scheduleCode":"MONTHLY","priceCompDetails":{"priceCompId":"5417300044","priceCompDesc":"FLAT","valueAmt":"3","displaySw":"true","rcMapId":"1705351562","tieredFlag":"FLAT","priceCompSequenceNo":"10"}}}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"modelId":"3488649738","dealId":"4538544755","entityType":"PERS","entityId":"8797366188","pricingAndCommitmentsDetails":{"entityDivision":"IND","entityIdentifierType":"COREG","entityType":"PERS","entityId":"8797366188","entityIdentifierValue":"Reg_BANK_82_EPER_001","pricingDetails":[{"txnDailyRatingCrt":"DNRT","priceCompDetails":{"priceCompId":"7658601072","valueAmt":"2","priceCompDesc":"FLAT","rcMapId":"1705351562","displaySw":"true","tieredFlag":"FLAT","priceCompSequenceNo":"10"},"parameterDetails":[{"parameterCode":"DM_CURRENCY","parameterValue":"INR"},{"parameterCode":"DM_TYPE","parameterValue":"BT"}],"paTypeFlag":"RGLR","priceItemDescription":"V8-Cheque Collections","aggregateSw":"N","priceItemCode":"PI_028","priceCurrencyCode":"USD","priceAsgnId":"7650014582","pricingStatus":"PRPD","printIfZero":"Y","ignoreSw":"N","actionFlag":"OVRD","isEligible":"false","scheduleCode":"MONTHLY","rateSchedule":"DM-RT01","startDate":"2023-09-11","assignmentLevel":"Customer Agreed"}]}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"dealId":"4538544755","modelId":"3488649738","entityId":"8797366188","entityType":"PERS","pricingAndCommitmentsDetails":{"entityId":"8797366188","entityType":"PERS","entityIdentifierValue":"Reg_BANK_82_EPER_001","entityIdentifierType":"COREG","entityDivision":"IND","pricingDetails":{"priceAsgnId":"7650014583","actionFlag":"OVRD","priceItemCode":"PI_028","priceItemDescription":"V8-Cheque Collections","pricingStatus":"PRPD","priceCurrencyCode":"USD","rateSchedule":"DM-RT01","startDate":"2023-09-11","isEligible":"false","assignmentLevel":"Customer Agreed","paTypeFlag":"RGLR","printIfZero":"Y","parameterDetails":[{"parameterCode":"DM_CURRENCY","parameterValue":"INR"},{"parameterCode":"DM_TYPE","parameterValue":"BT"}],"txnDailyRatingCrt":"DNRT","ignoreSw":"N","aggregateSw":"N","scheduleCode":"MONTHLY","priceCompDetails":{"priceCompId":"7658601072","priceCompDesc":"FLAT","valueAmt":"2","displaySw":"true","rcMapId":"1705351562","tieredFlag":"FLAT","priceCompSequenceNo":"10"}}}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"modelId":"3488649738","dealId":"4538544755","entityType":"PERS","entityId":"8797366188","pricingAndCommitmentsDetails":{"entityDivision":"IND","entityIdentifierType":"COREG","entityType":"PERS","entityId":"8797366188","entityIdentifierValue":"Reg_BANK_82_EPER_001","pricingDetails":[{"txnDailyRatingCrt":"DNRT","priceCompDetails":[{"priceCompId":"7658601055","valueAmt":"12","priceCompDesc":"Price Per Transaction Step Tier 1","rcMapId":"2567418376","displaySw":"true","tieredFlag":"STEP","priceCompTier":{"tierSeqNum":"10","upperLimit":"1000.00","lowerLimit":"0.00","priceCriteria":"NBRTRAN"},"priceCompSequenceNo":"100"},{"priceCompId":"7658601056","valueAmt":"13","priceCompDesc":"Price Per Transaction Step Tier 2","rcMapId":"7769990702","displaySw":"true","tieredFlag":"STEP","priceCompTier":{"tierSeqNum":"10","upperLimit":"5000.00","lowerLimit":"1000.00","priceCriteria":"NBRTRAN"},"priceCompSequenceNo":"110"},{"priceCompId":"7658601057","valueAmt":"14","priceCompDesc":"Price Per Transaction Step Tier 3","rcMapId":"4322456059","displaySw":"true","tieredFlag":"STEP","priceCompTier":{"tierSeqNum":"10","upperLimit":"99999999.99","lowerLimit":"5000.00","priceCriteria":"NBRTRAN"},"priceCompSequenceNo":"120"}],"parameterDetails":[{"parameterCode":"DM_COUNTRY","parameterValue":"IND"},{"parameterCode":"DM_STATE","parameterValue":"KA"}],"paTypeFlag":"RGLR","priceItemDescription":"Price Item NPI_036","aggregateSw":"N","priceItemCode":"NPI_036","priceCurrencyCode":"USD","priceAsgnId":"7650014575","pricingStatus":"PRPD","printIfZero":"Y","ignoreSw":"N","actionFlag":"UPD","isEligible":"false","scheduleCode":"MONTHLY","rateSchedule":"DM-NBRST","startDate":"2023-08-12","assignmentLevel":"Customer Agreed"}]}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"dealId":"4538544755","modelId":"3488649738","entityId":"8797366188","entityType":"PERS","pricingAndCommitmentsDetails":{"entityId":"8797366188","entityType":"PERS","entityIdentifierValue":"Reg_BANK_82_EPER_001","entityIdentifierType":"COREG","entityDivision":"IND","pricingDetails":{"priceAsgnId":"7650014575","actionFlag":"UPD","priceItemCode":"NPI_036","priceItemDescription":"Price Item NPI_036","pricingStatus":"PRPD","priceCurrencyCode":"USD","rateSchedule":"DM-NBRST","startDate":"2023-08-12","isEligible":"false","assignmentLevel":"Customer Agreed","paTypeFlag":"RGLR","printIfZero":"Y","parameterDetails":[{"parameterCode":"DM_COUNTRY","parameterValue":"IND"},{"parameterCode":"DM_STATE","parameterValue":"KA"}],"txnDailyRatingCrt":"DNRT","ignoreSw":"N","aggregateSw":"N","scheduleCode":"MONTHLY","priceCompDetails":[{"priceCompTier":{"upperLimit":"1000.00","lowerLimit":"0.00","priceCriteria":"NBRTRAN","tierSeqNum":"10"},"priceCompId":"7658601055","priceCompDesc":"Price Per Transaction Step Tier 1","valueAmt":"12","displaySw":"true","rcMapId":"2567418376","tieredFlag":"STEP","priceCompSequenceNo":"100"},{"priceCompTier":{"upperLimit":"5000.00","lowerLimit":"1000.00","priceCriteria":"NBRTRAN","tierSeqNum":"10"},"priceCompId":"7658601056","priceCompDesc":"Price Per Transaction Step Tier 2","valueAmt":"13","displaySw":"true","rcMapId":"7769990702","tieredFlag":"STEP","priceCompSequenceNo":"110"},{"priceCompTier":{"upperLimit":"99999999.99","lowerLimit":"5000.00","priceCriteria":"NBRTRAN","tierSeqNum":"10"},"priceCompId":"7658601057","priceCompDesc":"Price Per Transaction Step Tier 3","valueAmt":"14","displaySw":"true","rcMapId":"4322456059","tieredFlag":"STEP","priceCompSequenceNo":"120"}]}}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"modelId":"3488649738","dealId":"4538544755","entityType":"PERS","entityId":"8797366188","pricingAndCommitmentsDetails":{"entityDivision":"IND","entityIdentifierType":"COREG","entityType":"PERS","entityId":"8797366188","entityIdentifierValue":"Reg_BANK_82_EPER_001","pricingDetails":[{"txnDailyRatingCrt":"DNRT","priceCompDetails":[{"priceCompId":"7658601055","valueAmt":"11","priceCompDesc":"Price Per Transaction Step Tier 1","rcMapId":"2567418376","displaySw":"true","tieredFlag":"STEP","priceCompTier":{"tierSeqNum":"10","upperLimit":"1000.00","lowerLimit":"0.00","priceCriteria":"NBRTRAN"},"priceCompSequenceNo":"100"},{"priceCompId":"7658601056","valueAmt":"12","priceCompDesc":"Price Per Transaction Step Tier 2","rcMapId":"7769990702","displaySw":"true","tieredFlag":"STEP","priceCompTier":{"tierSeqNum":"10","upperLimit":"5000.00","lowerLimit":"1000.00","priceCriteria":"NBRTRAN"},"priceCompSequenceNo":"110"},{"priceCompId":"7658601057","valueAmt":"13","priceCompDesc":"Price Per Transaction Step Tier 3","rcMapId":"4322456059","displaySw":"true","tieredFlag":"STEP","priceCompTier":{"tierSeqNum":"10","upperLimit":"99999999.99","lowerLimit":"5000.00","priceCriteria":"NBRTRAN"},"priceCompSequenceNo":"120"}],"parameterDetails":[{"parameterCode":"DM_COUNTRY","parameterValue":"IND"},{"parameterCode":"DM_STATE","parameterValue":"KA"}],"paTypeFlag":"RGLR","priceItemDescription":"Price Item NPI_036","aggregateSw":"Y","priceItemCode":"NPI_036","priceCurrencyCode":"USD","priceAsgnId":"7650014575","pricingStatus":"PRPD","printIfZero":"Y","ignoreSw":"N","actionFlag":"OVRD","isEligible":"false","scheduleCode":"MONTHLY","rateSchedule":"DM-NBRST","startDate":"2023-09-11","assignmentLevel":"Customer Agreed"}]}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"dealId":"4538544755","modelId":"3488649738","entityId":"8797366188","entityType":"PERS","pricingAndCommitmentsDetails":{"entityId":"8797366188","entityType":"PERS","entityIdentifierValue":"Reg_BANK_82_EPER_001","entityIdentifierType":"COREG","entityDivision":"IND","pricingDetails":{"priceAsgnId":"7650014584","actionFlag":"OVRD","priceItemCode":"NPI_036","priceItemDescription":"Price Item NPI_036","pricingStatus":"PRPD","priceCurrencyCode":"USD","rateSchedule":"DM-NBRST","startDate":"2023-09-11","isEligible":"false","assignmentLevel":"Customer Agreed","paTypeFlag":"RGLR","printIfZero":"Y","parameterDetails":[{"parameterCode":"DM_COUNTRY","parameterValue":"IND"},{"parameterCode":"DM_STATE","parameterValue":"KA"}],"txnDailyRatingCrt":"DNRT","ignoreSw":"N","aggregateSw":"Y","scheduleCode":"MONTHLY","priceCompDetails":[{"priceCompTier":{"upperLimit":"1000.00","lowerLimit":"0.00","priceCriteria":"NBRTRAN","tierSeqNum":"10"},"priceCompId":"7658601055","priceCompDesc":"Price Per Transaction Step Tier 1","valueAmt":"11","displaySw":"true","rcMapId":"2567418376","tieredFlag":"STEP","priceCompSequenceNo":"100"},{"priceCompTier":{"upperLimit":"5000.00","lowerLimit":"1000.00","priceCriteria":"NBRTRAN","tierSeqNum":"10"},"priceCompId":"7658601056","priceCompDesc":"Price Per Transaction Step Tier 2","valueAmt":"12","displaySw":"true","rcMapId":"7769990702","tieredFlag":"STEP","priceCompSequenceNo":"110"},{"priceCompTier":{"upperLimit":"99999999.99","lowerLimit":"5000.00","priceCriteria":"NBRTRAN","tierSeqNum":"10"},"priceCompId":"7658601057","priceCompDesc":"Price Per Transaction Step Tier 3","valueAmt":"13","displaySw":"true","rcMapId":"4322456059","tieredFlag":"STEP","priceCompSequenceNo":"120"}]}}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"modelId":"3488649738","dealId":"4538544755","entityType":"PERS","entityId":"8797366188","pricingAndCommitmentsDetails":{"entityDivision":"IND","entityIdentifierType":"COREG","entityType":"PERS","entityId":"8797366188","entityIdentifierValue":"Reg_BANK_82_EPER_001","pricingDetails":[{"txnDailyRatingCrt":"DNRT","priceCompDetails":[{"priceCompId":"7658601052","valueAmt":"32","priceCompDesc":"Threshold price per transaction1","rcMapId":"1109655113","displaySw":"true","tieredFlag":"THRS","priceCompTier":{"tierSeqNum":"10","upperLimit":"1000.00","lowerLimit":"0.00","priceCriteria":"NBRTRAN"},"priceCompSequenceNo":"100"},{"priceCompId":"7658601053","valueAmt":"33","priceCompDesc":"Threshold price per transaction 2","rcMapId":"1109655113","displaySw":"true","tieredFlag":"THRS","priceCompTier":{"tierSeqNum":"10","upperLimit":"5000.00","lowerLimit":"1000.00","priceCriteria":"NBRTRAN"},"priceCompSequenceNo":"110"},{"priceCompId":"7658601054","valueAmt":"34","priceCompDesc":"Threshold price per transaction 3","rcMapId":"1109655113","displaySw":"true","tieredFlag":"THRS","priceCompTier":{"tierSeqNum":"10","upperLimit":"99999999.99","lowerLimit":"5000.00","priceCriteria":"NBRTRAN"},"priceCompSequenceNo":"120"}],"parameterDetails":[{"parameterCode":"DM_COUNTRY","parameterValue":"IND"},{"parameterCode":"DM_STATE","parameterValue":"AP"}],"paTypeFlag":"RGLR","priceItemDescription":"Price Item NPI_036","aggregateSw":"N","priceItemCode":"NPI_036","priceCurrencyCode":"USD","priceAsgnId":"7650014574","pricingStatus":"PRPD","printIfZero":"Y","ignoreSw":"N","actionFlag":"UPD","isEligible":"false","scheduleCode":"MONTHLY","rateSchedule":"DM-NBRTH","startDate":"2023-08-12","assignmentLevel":"Customer Agreed"}]}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"dealId":"4538544755","modelId":"3488649738","entityId":"8797366188","entityType":"PERS","pricingAndCommitmentsDetails":{"entityId":"8797366188","entityType":"PERS","entityIdentifierValue":"Reg_BANK_82_EPER_001","entityIdentifierType":"COREG","entityDivision":"IND","pricingDetails":{"priceAsgnId":"7650014574","actionFlag":"UPD","priceItemCode":"NPI_036","priceItemDescription":"Price Item NPI_036","pricingStatus":"PRPD","priceCurrencyCode":"USD","rateSchedule":"DM-NBRTH","startDate":"2023-08-12","isEligible":"false","assignmentLevel":"Customer Agreed","paTypeFlag":"RGLR","printIfZero":"Y","parameterDetails":[{"parameterCode":"DM_COUNTRY","parameterValue":"IND"},{"parameterCode":"DM_STATE","parameterValue":"AP"}],"txnDailyRatingCrt":"DNRT","ignoreSw":"N","aggregateSw":"N","scheduleCode":"MONTHLY","priceCompDetails":[{"priceCompTier":{"upperLimit":"1000.00","lowerLimit":"0.00","priceCriteria":"NBRTRAN","tierSeqNum":"10"},"priceCompId":"7658601052","priceCompDesc":"Threshold price per transaction1","valueAmt":"32","displaySw":"true","rcMapId":"1109655113","tieredFlag":"THRS","priceCompSequenceNo":"100"},{"priceCompTier":{"upperLimit":"5000.00","lowerLimit":"1000.00","priceCriteria":"NBRTRAN","tierSeqNum":"10"},"priceCompId":"7658601053","priceCompDesc":"Threshold price per transaction 2","valueAmt":"33","displaySw":"true","rcMapId":"1109655113","tieredFlag":"THRS","priceCompSequenceNo":"110"},{"priceCompTier":{"upperLimit":"99999999.99","lowerLimit":"5000.00","priceCriteria":"NBRTRAN","tierSeqNum":"10"},"priceCompId":"7658601054","priceCompDesc":"Threshold price per transaction 3","valueAmt":"34","displaySw":"true","rcMapId":"1109655113","tieredFlag":"THRS","priceCompSequenceNo":"120"}]}}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"modelId":"3488649738","dealId":"4538544755","entityType":"PERS","entityId":"8797366188","pricingAndCommitmentsDetails":{"entityDivision":"IND","entityIdentifierType":"COREG","entityType":"PERS","entityId":"8797366188","entityIdentifierValue":"Reg_BANK_82_EPER_001","pricingDetails":[{"txnDailyRatingCrt":"DNRT","priceCompDetails":[{"priceCompId":"7658601052","valueAmt":"31","priceCompDesc":"Threshold price per transaction1","rcMapId":"1109655113","displaySw":"true","tieredFlag":"THRS","priceCompTier":{"tierSeqNum":"10","upperLimit":"1000.00","lowerLimit":"0.00","priceCriteria":"NBRTRAN"},"priceCompSequenceNo":"100"},{"priceCompId":"7658601053","valueAmt":"32","priceCompDesc":"Threshold price per transaction 2","rcMapId":"1109655113","displaySw":"true","tieredFlag":"THRS","priceCompTier":{"tierSeqNum":"10","upperLimit":"5000.00","lowerLimit":"1000.00","priceCriteria":"NBRTRAN"},"priceCompSequenceNo":"110"},{"priceCompId":"7658601054","valueAmt":"33","priceCompDesc":"Threshold price per transaction 3","rcMapId":"1109655113","displaySw":"true","tieredFlag":"THRS","priceCompTier":{"tierSeqNum":"10","upperLimit":"99999999.99","lowerLimit":"5000.00","priceCriteria":"NBRTRAN"},"priceCompSequenceNo":"120"}],"parameterDetails":[{"parameterCode":"DM_COUNTRY","parameterValue":"IND"},{"parameterCode":"DM_STATE","parameterValue":"AP"}],"paTypeFlag":"RGLR","priceItemDescription":"Price Item NPI_036","aggregateSw":"Y","priceItemCode":"NPI_036","priceCurrencyCode":"USD","priceAsgnId":"7650014574","pricingStatus":"PRPD","printIfZero":"Y","ignoreSw":"N","actionFlag":"OVRD","isEligible":"false","scheduleCode":"MONTHLY","rateSchedule":"DM-NBRTH","startDate":"2023-09-11","assignmentLevel":"Customer Agreed"}]}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"dealId":"4538544755","modelId":"3488649738","entityId":"8797366188","entityType":"PERS","pricingAndCommitmentsDetails":{"entityId":"8797366188","entityType":"PERS","entityIdentifierValue":"Reg_BANK_82_EPER_001","entityIdentifierType":"COREG","entityDivision":"IND","pricingDetails":{"priceAsgnId":"7650014585","actionFlag":"OVRD","priceItemCode":"NPI_036","priceItemDescription":"Price Item NPI_036","pricingStatus":"PRPD","priceCurrencyCode":"USD","rateSchedule":"DM-NBRTH","startDate":"2023-09-11","isEligible":"false","assignmentLevel":"Customer Agreed","paTypeFlag":"RGLR","printIfZero":"Y","parameterDetails":[{"parameterCode":"DM_COUNTRY","parameterValue":"IND"},{"parameterCode":"DM_STATE","parameterValue":"AP"}],"txnDailyRatingCrt":"DNRT","ignoreSw":"N","aggregateSw":"Y","scheduleCode":"MONTHLY","priceCompDetails":[{"priceCompTier":{"upperLimit":"1000.00","lowerLimit":"0.00","priceCriteria":"NBRTRAN","tierSeqNum":"10"},"priceCompId":"7658601052","priceCompDesc":"Threshold price per transaction1","valueAmt":"31","displaySw":"true","rcMapId":"1109655113","tieredFlag":"THRS","priceCompSequenceNo":"100"},{"priceCompTier":{"upperLimit":"5000.00","lowerLimit":"1000.00","priceCriteria":"NBRTRAN","tierSeqNum":"10"},"priceCompId":"7658601053","priceCompDesc":"Threshold price per transaction 2","valueAmt":"32","displaySw":"true","rcMapId":"1109655113","tieredFlag":"THRS","priceCompSequenceNo":"110"},{"priceCompTier":{"upperLimit":"99999999.99","lowerLimit":"5000.00","priceCriteria":"NBRTRAN","tierSeqNum":"10"},"priceCompId":"7658601054","priceCompDesc":"Threshold price per transaction 3","valueAmt":"33","displaySw":"true","rcMapId":"1109655113","tieredFlag":"THRS","priceCompSequenceNo":"120"}]}}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"modelId":"3488649738","dealId":"4538544755","entityType":"PERS","entityId":"8797366188","pricingAndCommitmentsDetails":{"entityDivision":"IND","entityIdentifierType":"COREG","entityType":"PERS","entityId":"8797366188","entityIdentifierValue":"Reg_BANK_82_EPER_001","pricingDetails":[{"txnDailyRatingCrt":"DNRT","priceCompDetails":{"priceCompId":"5417300002","valueAmt":"11","priceCompDesc":"FLAT","rcMapId":"1705351562","displaySw":"true","tieredFlag":"FLAT","priceCompSequenceNo":"10"},"paTypeFlag":"RGLR","priceItemDescription":"MT943_SWIFT_01","aggregateSw":"Y","priceItemCode":"PI_031","priceCurrencyCode":"USD","priceAsgnId":"5410009201","pricingStatus":"PRPD","printIfZero":"Y","ignoreSw":"N","actionFlag":"OVRD","isEligible":"false","scheduleCode":"MONTHLY","rateSchedule":"DM-RT01","startDate":"2023-08-12","assignmentLevel":"Customer Price List"}]}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"dealId":"4538544755","modelId":"3488649738","entityId":"8797366188","entityType":"PERS","pricingAndCommitmentsDetails":{"entityId":"8797366188","entityType":"PERS","entityIdentifierValue":"Reg_BANK_82_EPER_001","entityIdentifierType":"COREG","entityDivision":"IND","pricingDetails":{"priceAsgnId":"7650014586","actionFlag":"OVRD","priceItemCode":"PI_031","priceItemDescription":"MT943_SWIFT_01","pricingStatus":"PRPD","priceCurrencyCode":"USD","rateSchedule":"DM-RT01","startDate":"2023-08-12","isEligible":"false","assignmentLevel":"Customer Price List","paTypeFlag":"RGLR","printIfZero":"Y","txnDailyRatingCrt":"DNRT","ignoreSw":"N","aggregateSw":"Y","scheduleCode":"MONTHLY","priceCompDetails":{"priceCompId":"5417300002","priceCompDesc":"FLAT","valueAmt":"11","displaySw":"true","rcMapId":"1705351562","tieredFlag":"FLAT","priceCompSequenceNo":"10"}}}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"modelId":"3488649738","dealId":"4538544755","entityType":"PERS","entityId":"8797366188","pricingAndCommitmentsDetails":{"entityDivision":"IND","entityIdentifierType":"COREG","entityType":"PERS","entityId":"8797366188","entityIdentifierValue":"Reg_BANK_82_EPER_001","pricingDetails":[{"txnDailyRatingCrt":"DNRT","priceCompDetails":{"priceCompId":"7658601080","valueAmt":"12","priceCompDesc":"FLAT","rcMapId":"1705351562","displaySw":"true","tieredFlag":"FLAT","priceCompSequenceNo":"10"},"paTypeFlag":"RGLR","priceItemDescription":"MT943_SWIFT_01","aggregateSw":"N","priceItemCode":"PI_031","priceCurrencyCode":"USD","priceAsgnId":"7650014586","pricingStatus":"PRPD","printIfZero":"Y","ignoreSw":"N","actionFlag":"OVRD","isEligible":"false","scheduleCode":"MONTHLY","rateSchedule":"DM-RT01","startDate":"2023-09-11","assignmentLevel":"Customer Agreed"}]}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"dealId":"4538544755","modelId":"3488649738","entityId":"8797366188","entityType":"PERS","pricingAndCommitmentsDetails":{"entityId":"8797366188","entityType":"PERS","entityIdentifierValue":"Reg_BANK_82_EPER_001","entityIdentifierType":"COREG","entityDivision":"IND","pricingDetails":{"priceAsgnId":"7650014587","actionFlag":"OVRD","priceItemCode":"PI_031","priceItemDescription":"MT943_SWIFT_01","pricingStatus":"PRPD","priceCurrencyCode":"USD","rateSchedule":"DM-RT01","startDate":"2023-09-11","isEligible":"false","assignmentLevel":"Customer Agreed","paTypeFlag":"RGLR","printIfZero":"Y","txnDailyRatingCrt":"DNRT","ignoreSw":"N","aggregateSw":"N","scheduleCode":"MONTHLY","priceCompDetails":{"priceCompId":"7658601080","priceCompDesc":"FLAT","valueAmt":"12","displaySw":"true","rcMapId":"1705351562","tieredFlag":"FLAT","priceCompSequenceNo":"10"}}}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"modelId":"3488649738","dealId":"4538544755","entityType":"PERS","entityId":"8797366188","pricingAndCommitmentsDetails":{"entityDivision":"IND","entityIdentifierType":"COREG","entityType":"PERS","entityId":"8797366188","entityIdentifierValue":"Reg_BANK_82_EPER_001","pricingDetails":[{"txnDailyRatingCrt":"DNRT","priceCompDetails":{"priceCompId":"5417300038","valueAmt":"777","priceCompDesc":"Basic BK-NBR","rcMapId":"9384470053","displaySw":"true","tieredFlag":"FLAT","priceCompSequenceNo":"10"},"paTypeFlag":"RGLR","priceItemDescription":"V7-Direct Debit","aggregateSw":"Y","priceItemCode":"PI_027","priceCurrencyCode":"USD","priceAsgnId":"5410009209","pricingStatus":"PRPD","printIfZero":"Y","ignoreSw":"N","actionFlag":"OVRD","isEligible":"false","scheduleCode":"MONTHLY","rateSchedule":"DM-RT03","startDate":"2023-08-12","assignmentLevel":"Customer Price List"}]}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"dealId":"4538544755","modelId":"3488649738","entityId":"8797366188","entityType":"PERS","pricingAndCommitmentsDetails":{"entityId":"8797366188","entityType":"PERS","entityIdentifierValue":"Reg_BANK_82_EPER_001","entityIdentifierType":"COREG","entityDivision":"IND","pricingDetails":{"priceAsgnId":"7650014588","actionFlag":"OVRD","priceItemCode":"PI_027","priceItemDescription":"V7-Direct Debit","pricingStatus":"PRPD","priceCurrencyCode":"USD","rateSchedule":"DM-RT03","startDate":"2023-08-12","isEligible":"false","assignmentLevel":"Customer Price List","paTypeFlag":"RGLR","printIfZero":"Y","txnDailyRatingCrt":"DNRT","ignoreSw":"N","aggregateSw":"Y","scheduleCode":"MONTHLY","priceCompDetails":{"priceCompId":"5417300038","priceCompDesc":"Basic BK-NBR","valueAmt":"777","displaySw":"true","rcMapId":"9384470053","tieredFlag":"FLAT","priceCompSequenceNo":"10"}}}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"modelId":"3488649738","dealId":"4538544755","entityType":"PERS","entityId":"8797366188","pricingAndCommitmentsDetails":{"entityDivision":"IND","entityIdentifierType":"COREG","entityType":"PERS","entityId":"8797366188","entityIdentifierValue":"Reg_BANK_82_EPER_001","pricingDetails":[{"txnDailyRatingCrt":"DNRT","priceCompDetails":{"priceCompId":"7658601082","valueAmt":"775","priceCompDesc":"Basic BK-NBR","rcMapId":"9384470053","displaySw":"true","tieredFlag":"FLAT","priceCompSequenceNo":"10"},"paTypeFlag":"RGLR","priceItemDescription":"V7-Direct Debit","aggregateSw":"N","priceItemCode":"PI_027","priceCurrencyCode":"USD","priceAsgnId":"7650014588","pricingStatus":"PRPD","printIfZero":"Y","ignoreSw":"N","actionFlag":"OVRD","isEligible":"false","scheduleCode":"MONTHLY","rateSchedule":"DM-RT03","startDate":"2023-09-11","assignmentLevel":"Customer Agreed"}]}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"dealId":"4538544755","modelId":"3488649738","entityId":"8797366188","entityType":"PERS","pricingAndCommitmentsDetails":{"entityId":"8797366188","entityType":"PERS","entityIdentifierValue":"Reg_BANK_82_EPER_001","entityIdentifierType":"COREG","entityDivision":"IND","pricingDetails":{"priceAsgnId":"7650014589","actionFlag":"OVRD","priceItemCode":"PI_027","priceItemDescription":"V7-Direct Debit","pricingStatus":"PRPD","priceCurrencyCode":"USD","rateSchedule":"DM-RT03","startDate":"2023-09-11","isEligible":"false","assignmentLevel":"Customer Agreed","paTypeFlag":"RGLR","printIfZero":"Y","txnDailyRatingCrt":"DNRT","ignoreSw":"N","aggregateSw":"N","scheduleCode":"MONTHLY","priceCompDetails":{"priceCompId":"7658601082","priceCompDesc":"Basic BK-NBR","valueAmt":"775","displaySw":"true","rcMapId":"9384470053","tieredFlag":"FLAT","priceCompSequenceNo":"10"}}}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"modelId":"3488649738","dealId":"4538544755","entityType":"PERS","entityId":"8797366188","pricingAndCommitmentsDetails":{"entityDivision":"IND","entityIdentifierType":"COREG","entityType":"PERS","entityId":"8797366188","entityIdentifierValue":"Reg_BANK_82_EPER_001","pricingDetails":[{"txnDailyRatingCrt":"DNRT","priceCompDetails":{"priceCompId":"5417300004","valueAmt":"13","priceCompDesc":"FLAT","rcMapId":"1705351562","displaySw":"true","tieredFlag":"FLAT","priceCompSequenceNo":"10"},"paTypeFlag":"RGLR","priceItemDescription":"V1-Account Opening Fee","aggregateSw":"Y","priceItemCode":"PI_021","priceCurrencyCode":"USD","priceAsgnId":"5410009202","pricingStatus":"PRPD","printIfZero":"Y","ignoreSw":"N","actionFlag":"OVRD","isEligible":"false","scheduleCode":"MONTHLY","rateSchedule":"DM-RT01","startDate":"2023-08-12","assignmentLevel":"Customer Price List"}]}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"dealId":"4538544755","modelId":"3488649738","entityId":"8797366188","entityType":"PERS","pricingAndCommitmentsDetails":{"entityId":"8797366188","entityType":"PERS","entityIdentifierValue":"Reg_BANK_82_EPER_001","entityIdentifierType":"COREG","entityDivision":"IND","pricingDetails":{"priceAsgnId":"7650014590","actionFlag":"OVRD","priceItemCode":"PI_021","priceItemDescription":"V1-Account Opening Fee","pricingStatus":"PRPD","priceCurrencyCode":"USD","rateSchedule":"DM-RT01","startDate":"2023-08-12","isEligible":"false","assignmentLevel":"Customer Price List","paTypeFlag":"RGLR","printIfZero":"Y","txnDailyRatingCrt":"DNRT","ignoreSw":"N","aggregateSw":"Y","scheduleCode":"MONTHLY","priceCompDetails":{"priceCompId":"5417300004","priceCompDesc":"FLAT","valueAmt":"13","displaySw":"true","rcMapId":"1705351562","tieredFlag":"FLAT","priceCompSequenceNo":"10"}}}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"modelId":"3488649738","dealId":"4538544755","entityType":"PERS","entityId":"8797366188","pricingAndCommitmentsDetails":{"entityDivision":"IND","entityIdentifierType":"COREG","entityType":"PERS","entityId":"8797366188","entityIdentifierValue":"Reg_BANK_82_EPER_001","pricingDetails":[{"txnDailyRatingCrt":"DNRT","priceCompDetails":{"priceCompId":"7658601084","valueAmt":"12","priceCompDesc":"FLAT","rcMapId":"1705351562","displaySw":"true","tieredFlag":"FLAT","priceCompSequenceNo":"10"},"paTypeFlag":"RGLR","priceItemDescription":"V1-Account Opening Fee","aggregateSw":"N","priceItemCode":"PI_021","priceCurrencyCode":"USD","priceAsgnId":"7650014590","pricingStatus":"PRPD","printIfZero":"Y","ignoreSw":"N","actionFlag":"OVRD","isEligible":"false","scheduleCode":"MONTHLY","rateSchedule":"DM-RT01","startDate":"2023-09-11","assignmentLevel":"Customer Agreed"}]}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"dealId":"4538544755","modelId":"3488649738","entityId":"8797366188","entityType":"PERS","pricingAndCommitmentsDetails":{"entityId":"8797366188","entityType":"PERS","entityIdentifierValue":"Reg_BANK_82_EPER_001","entityIdentifierType":"COREG","entityDivision":"IND","pricingDetails":{"priceAsgnId":"7650014591","actionFlag":"OVRD","priceItemCode":"PI_021","priceItemDescription":"V1-Account Opening Fee","pricingStatus":"PRPD","priceCurrencyCode":"USD","rateSchedule":"DM-RT01","startDate":"2023-09-11","isEligible":"false","assignmentLevel":"Customer Agreed","paTypeFlag":"RGLR","printIfZero":"Y","txnDailyRatingCrt":"DNRT","ignoreSw":"N","aggregateSw":"N","scheduleCode":"MONTHLY","priceCompDetails":{"priceCompId":"7658601084","priceCompDesc":"FLAT","valueAmt":"12","displaySw":"true","rcMapId":"1705351562","tieredFlag":"FLAT","priceCompSequenceNo":"10"}}}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"modelId":"3488649738","dealId":"4538544755","entityType":"PERS","entityId":"8797366188","pricingAndCommitmentsDetails":{"entityDivision":"IND","entityIdentifierType":"COREG","entityType":"PERS","entityId":"8797366188","entityIdentifierValue":"Reg_BANK_82_EPER_001","pricingDetails":[{"txnDailyRatingCrt":"DNRT","priceCompDetails":{"priceCompId":"7658601050","valueAmt":"12","priceCompDesc":"Basic","rcMapId":"1705351562","displaySw":"true","tieredFlag":"FLAT","priceCompSequenceNo":"10"},"paTypeFlag":"RGLR","priceItemDescription":"Price Item NPI_024","aggregateSw":"N","priceItemCode":"NPI_024","priceCurrencyCode":"USD","priceAsgnId":"7650014572","pricingStatus":"RECM","printIfZero":"Y","ignoreSw":"N","actionFlag":"RECM","isEligible":"false","scheduleCode":"MONTHLY","rateSchedule":"DM-RT01","startDate":"2020-01-01","assignmentLevel":"Customer Agreed"}]}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"dealId":"4538544755","modelId":"3488649738","entityId":"8797366188","entityType":"PERS","pricingAndCommitmentsDetails":{"entityId":"8797366188","entityType":"PERS","entityIdentifierValue":"Reg_BANK_82_EPER_001","entityIdentifierType":"COREG","entityDivision":"IND","pricingDetails":{"priceAsgnId":"7650014592","actionFlag":"RECM","priceItemCode":"NPI_024","priceItemDescription":"Price Item NPI_024","pricingStatus":"RECM","priceCurrencyCode":"USD","rateSchedule":"DM-RT01","startDate":"2020-01-01","isEligible":"false","assignmentLevel":"Customer Agreed","paTypeFlag":"RGLR","printIfZero":"Y","txnDailyRatingCrt":"DNRT","ignoreSw":"N","aggregateSw":"N","scheduleCode":"MONTHLY","priceCompDetails":{"priceCompId":"7658601050","priceCompDesc":"Basic","valueAmt":"12","displaySw":"true","rcMapId":"1705351562","tieredFlag":"FLAT","priceCompSequenceNo":"10"}}}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"modelId":"3488649738","dealId":"4538544755","entityType":"PERS","entityId":"8797366188","pricingAndCommitmentsDetails":{"entityDivision":"IND","entityIdentifierType":"COREG","entityType":"PERS","entityId":"8797366188","entityIdentifierValue":"Reg_BANK_82_EPER_001","pricingDetails":[{"txnDailyRatingCrt":"DNRT","priceCompDetails":{"priceCompId":"7658601050","valueAmt":"12","priceCompDesc":"Basic","rcMapId":"1705351562","displaySw":"true","tieredFlag":"FLAT","priceCompSequenceNo":"10"},"paTypeFlag":"RGLR","priceItemDescription":"Price Item NPI_024","aggregateSw":"N","priceItemCode":"NPI_024","priceCurrencyCode":"USD","priceAsgnId":"7650014572","pricingStatus":"PRPD","printIfZero":"Y","ignoreSw":"N","actionFlag":"UPD","isEligible":"false","scheduleCode":"MONTHLY","rateSchedule":"DM-RT01","startDate":"2020-01-01","assignmentLevel":"Customer Agreed"}]}}}</t>
+  </si>
+  <si>
+    <t>{"C1-DealPriceAsgnCommitmentsREST":{"dealId":"4538544755","modelId":"3488649738","entityId":"8797366188","entityType":"PERS","pricingAndCommitmentsDetails":{"entityId":"8797366188","entityType":"PERS","entityIdentifierValue":"Reg_BANK_82_EPER_001","entityIdentifierType":"COREG","entityDivision":"IND","pricingDetails":{"priceAsgnId":"7650014572","actionFlag":"UPD","priceItemCode":"NPI_024","priceItemDescription":"Price Item NPI_024","pricingStatus":"PRPD","priceCurrencyCode":"USD","rateSchedule":"DM-RT01","startDate":"2020-01-01","isEligible":"false","assignmentLevel":"Customer Agreed","paTypeFlag":"RGLR","printIfZero":"Y","txnDailyRatingCrt":"DNRT","ignoreSw":"N","aggregateSw":"N","scheduleCode":"MONTHLY","priceCompDetails":{"priceCompId":"7658601050","priceCompDesc":"Basic","valueAmt":"12","displaySw":"true","rcMapId":"1705351562","tieredFlag":"FLAT","priceCompSequenceNo":"10"}}}}}</t>
   </si>
 </sst>
 </file>
@@ -8865,10 +9105,10 @@
       </c>
       <c r="Z124" s="81"/>
       <c r="AU124" t="s">
-        <v>591</v>
+        <v>671</v>
       </c>
       <c r="AV124" t="s">
-        <v>592</v>
+        <v>672</v>
       </c>
     </row>
     <row r="125" spans="1:48" x14ac:dyDescent="0.35">
@@ -8944,10 +9184,10 @@
       </c>
       <c r="Z125" s="86"/>
       <c r="AU125" t="s">
-        <v>593</v>
+        <v>673</v>
       </c>
       <c r="AV125" t="s">
-        <v>594</v>
+        <v>674</v>
       </c>
     </row>
     <row r="126" spans="1:48" x14ac:dyDescent="0.35">
@@ -9206,10 +9446,10 @@
       <c r="Y130" s="81"/>
       <c r="Z130" s="81"/>
       <c r="AU130" t="s">
-        <v>595</v>
+        <v>675</v>
       </c>
       <c r="AV130" t="s">
-        <v>596</v>
+        <v>676</v>
       </c>
     </row>
     <row r="131" spans="1:48" ht="19" customHeight="1" x14ac:dyDescent="0.35">
@@ -9279,10 +9519,10 @@
       <c r="Y131" s="86"/>
       <c r="Z131" s="86"/>
       <c r="AU131" t="s">
-        <v>597</v>
+        <v>677</v>
       </c>
       <c r="AV131" t="s">
-        <v>598</v>
+        <v>678</v>
       </c>
     </row>
     <row r="132" spans="1:48" ht="19" customHeight="1" x14ac:dyDescent="0.35">
@@ -9535,10 +9775,10 @@
       <c r="Y136" s="81"/>
       <c r="Z136" s="81"/>
       <c r="AU136" t="s">
-        <v>599</v>
+        <v>679</v>
       </c>
       <c r="AV136" t="s">
-        <v>600</v>
+        <v>680</v>
       </c>
     </row>
     <row r="137" spans="1:48" ht="19" customHeight="1" x14ac:dyDescent="0.35">
@@ -9608,10 +9848,10 @@
       <c r="Y137" s="86"/>
       <c r="Z137" s="86"/>
       <c r="AU137" t="s">
-        <v>601</v>
+        <v>681</v>
       </c>
       <c r="AV137" t="s">
-        <v>602</v>
+        <v>682</v>
       </c>
     </row>
     <row r="138" spans="1:48" ht="19" customHeight="1" x14ac:dyDescent="0.35">
@@ -9870,10 +10110,10 @@
       </c>
       <c r="Z142" s="81"/>
       <c r="AU142" t="s">
-        <v>603</v>
+        <v>683</v>
       </c>
       <c r="AV142" t="s">
-        <v>604</v>
+        <v>684</v>
       </c>
     </row>
     <row r="143" spans="1:48" ht="16" customHeight="1" x14ac:dyDescent="0.35">
@@ -9949,10 +10189,10 @@
       </c>
       <c r="Z143" s="86"/>
       <c r="AU143" t="s">
-        <v>605</v>
+        <v>685</v>
       </c>
       <c r="AV143" t="s">
-        <v>606</v>
+        <v>686</v>
       </c>
     </row>
     <row r="144" spans="1:48" ht="16" customHeight="1" x14ac:dyDescent="0.35">
@@ -10203,10 +10443,10 @@
       </c>
       <c r="Z148" s="90"/>
       <c r="AU148" t="s">
-        <v>607</v>
+        <v>687</v>
       </c>
       <c r="AV148" t="s">
-        <v>608</v>
+        <v>688</v>
       </c>
     </row>
     <row r="149" spans="1:48" ht="16" customHeight="1" x14ac:dyDescent="0.35">
@@ -10268,10 +10508,10 @@
       </c>
       <c r="Z149" s="86"/>
       <c r="AU149" t="s">
-        <v>609</v>
+        <v>689</v>
       </c>
       <c r="AV149" t="s">
-        <v>610</v>
+        <v>690</v>
       </c>
     </row>
     <row r="151" spans="1:48" ht="16" customHeight="1" x14ac:dyDescent="0.35">
@@ -10333,10 +10573,10 @@
       </c>
       <c r="Z151" s="90"/>
       <c r="AU151" t="s">
-        <v>611</v>
+        <v>691</v>
       </c>
       <c r="AV151" t="s">
-        <v>612</v>
+        <v>692</v>
       </c>
     </row>
     <row r="152" spans="1:48" ht="16" customHeight="1" x14ac:dyDescent="0.35">
@@ -10398,10 +10638,10 @@
       </c>
       <c r="Z152" s="86"/>
       <c r="AU152" t="s">
-        <v>613</v>
+        <v>693</v>
       </c>
       <c r="AV152" t="s">
-        <v>614</v>
+        <v>694</v>
       </c>
     </row>
     <row r="154" spans="1:48" x14ac:dyDescent="0.35">
@@ -10580,10 +10820,10 @@
       </c>
       <c r="Z156" s="81"/>
       <c r="AU156" t="s">
-        <v>615</v>
+        <v>695</v>
       </c>
       <c r="AV156" t="s">
-        <v>616</v>
+        <v>696</v>
       </c>
     </row>
     <row r="157" spans="1:48" ht="19" customHeight="1" x14ac:dyDescent="0.35">
@@ -10652,10 +10892,10 @@
       </c>
       <c r="Z157" s="86"/>
       <c r="AU157" t="s">
-        <v>617</v>
+        <v>697</v>
       </c>
       <c r="AV157" t="s">
-        <v>618</v>
+        <v>698</v>
       </c>
     </row>
     <row r="159" spans="1:48" x14ac:dyDescent="0.35">
@@ -10834,10 +11074,10 @@
       </c>
       <c r="Z161" s="81"/>
       <c r="AU161" t="s">
-        <v>619</v>
+        <v>699</v>
       </c>
       <c r="AV161" t="s">
-        <v>620</v>
+        <v>700</v>
       </c>
     </row>
     <row r="162" spans="1:48" ht="19" customHeight="1" x14ac:dyDescent="0.35">
@@ -10906,10 +11146,10 @@
       </c>
       <c r="Z162" s="86"/>
       <c r="AU162" t="s">
-        <v>621</v>
+        <v>701</v>
       </c>
       <c r="AV162" t="s">
-        <v>622</v>
+        <v>702</v>
       </c>
     </row>
     <row r="164" spans="1:48" x14ac:dyDescent="0.35">
@@ -11080,10 +11320,10 @@
       </c>
       <c r="Z166" s="81"/>
       <c r="AU166" t="s">
-        <v>623</v>
+        <v>703</v>
       </c>
       <c r="AV166" t="s">
-        <v>624</v>
+        <v>704</v>
       </c>
     </row>
     <row r="167" spans="1:48" ht="19" customHeight="1" x14ac:dyDescent="0.35">
@@ -11144,10 +11384,10 @@
       </c>
       <c r="Z167" s="86"/>
       <c r="AU167" t="s">
-        <v>625</v>
+        <v>705</v>
       </c>
       <c r="AV167" t="s">
-        <v>626</v>
+        <v>706</v>
       </c>
     </row>
     <row r="169" spans="1:48" x14ac:dyDescent="0.35">
@@ -12378,10 +12618,10 @@
       </c>
       <c r="Z202" s="81"/>
       <c r="AU202" t="s">
-        <v>627</v>
+        <v>707</v>
       </c>
       <c r="AV202" t="s">
-        <v>628</v>
+        <v>708</v>
       </c>
     </row>
     <row r="203" spans="1:78" ht="16" customHeight="1" x14ac:dyDescent="0.35">
@@ -12434,10 +12674,10 @@
       </c>
       <c r="Z203" s="81"/>
       <c r="AU203" t="s">
-        <v>629</v>
+        <v>709</v>
       </c>
       <c r="AV203" t="s">
-        <v>630</v>
+        <v>710</v>
       </c>
     </row>
     <row r="205" spans="1:78" x14ac:dyDescent="0.35">

</xml_diff>